<commit_message>
02/28 kernel launch analysis
</commit_message>
<xml_diff>
--- a/batch_size_test.xlsx
+++ b/batch_size_test.xlsx
@@ -4,61 +4,96 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.5152"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="22788" windowHeight="8664" tabRatio="535"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="18168" windowHeight="8664" tabRatio="626" activeTab="5"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <x:sheet name="02.25 persistent loop" sheetId="1" r:id="rId4"/>
     <x:sheet name="02.26 memcpy test" sheetId="2" r:id="rId5"/>
     <x:sheet name="02.27 memcpy test" sheetId="3" r:id="rId6"/>
     <x:sheet name="02.27 memcpy test graph" sheetId="4" r:id="rId7"/>
+    <x:sheet name="02.28 kernel launch" sheetId="5" r:id="rId8"/>
+    <x:sheet name="02.28 kernel launch graph" sheetId="6" r:id="rId9"/>
   </x:sheets>
   <x:calcPr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" mc:Ignorable="hs" hs:hclCalcId="904"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="32">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="33">
   <x:si>
-    <x:t>100 times loop / normal data</x:t>
+    <x:t>64 * 1024</x:t>
   </x:si>
   <x:si>
-    <x:t>same size loop / normal data</x:t>
+    <x:t>64 * 512</x:t>
   </x:si>
   <x:si>
-    <x:t>same size loop / random data</x:t>
-  </x:si>
-  <x:si>
-    <x:t>packet size별 batch size에 따른 pps</x:t>
+    <x:t>64 * 256</x:t>
   </x:si>
   <x:si>
     <x:t>64 * 128</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 512</x:t>
+    <x:t>64 * 1024 * 4</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 1024</x:t>
+    <x:t>256 (4.5Mpps)</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 256</x:t>
+    <x:t>Ascending Order</x:t>
   </x:si>
   <x:si>
-    <x:t>100times loop / random data</x:t>
+    <x:t>64 * 1024 * 8</x:t>
   </x:si>
   <x:si>
-    <x:t>1024*16</x:t>
+    <x:t>64 * 1024 * 32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>512 (2.35Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>128 (8.4Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 * 1024 * 16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1024 (1.2Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 * 1024 * 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1514 (0.8 Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>packet size별 batch size에 따른 cudaMemcpy call 횟수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>once / random data</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 (13.8~14.0Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>once / normal data</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Descending Order</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1024*2</x:t>
   </x:si>
   <x:si>
     <x:t>1024*4</x:t>
   </x:si>
   <x:si>
+    <x:t>64 * 64</x:t>
+  </x:si>
+  <x:si>
     <x:t>1024*8</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 64</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1024*2</x:t>
+    <x:t>1024*16</x:t>
   </x:si>
   <x:si>
     <x:t>64 * 32</x:t>
@@ -67,52 +102,22 @@
     <x:t>1024*32</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 1024 * 16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ascending Order</x:t>
-  </x:si>
-  <x:si>
-    <x:t>128 (8.4Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64 * 1024 * 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64 * 1024 * 8</x:t>
+    <x:t>100times loop / random data</x:t>
   </x:si>
   <x:si>
     <x:t>packet size별 batch size에 따른 rx rate</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 1024 * 32</x:t>
+    <x:t>same size loop / normal data</x:t>
   </x:si>
   <x:si>
-    <x:t>1024 (1.2Mpps)</x:t>
+    <x:t>100 times loop / normal data</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 1024 * 4</x:t>
+    <x:t>same size loop / random data</x:t>
   </x:si>
   <x:si>
-    <x:t>1514 (0.8 Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>256 (4.5Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>512 (2.35Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Descending Order</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64 (13.8~14.0Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>once / random data</x:t>
-  </x:si>
-  <x:si>
-    <x:t>once / normal data</x:t>
+    <x:t>packet size별 batch size에 따른 pps</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -364,7 +369,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -447,7 +451,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -482,7 +485,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -527,7 +529,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -571,7 +572,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -655,8 +655,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
+            <x:color indexed="64"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -667,6 +667,7 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
+            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
         </x:dxf>
@@ -676,8 +677,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
+            <x:color indexed="64"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -693,6 +694,7 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
+            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
           <x:border>
@@ -707,8 +709,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
+            <x:color indexed="64"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -724,6 +726,7 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
+            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
           <x:border>
@@ -761,7 +764,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1425,7 +1428,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1809,7 +1812,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2512,7 +2515,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2933,7 +2936,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3636,7 +3639,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -4057,7 +4060,1641 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <c:date1904 val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:p>
+            <a:pPr algn="l">
+              <a:defRPr sz="2000" b="1" i="0" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="함초롬돋움" panose="0"/>
+                <a:ea typeface="함초롬돋움" panose="0"/>
+                <a:cs typeface="함초롬돋움" panose="0"/>
+                <a:sym typeface="함초롬돋움" panose="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="2000" b="1" i="0" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="함초롬돋움" panose="0"/>
+                <a:ea typeface="함초롬돋움" panose="0"/>
+                <a:cs typeface="함초롬돋움" panose="0"/>
+                <a:sym typeface="함초롬돋움" panose="0"/>
+              </a:rPr>
+              <a:t>pps test with kernel launch</a:t>
+            </a:r>
+            <a:endParaRPr/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$21:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0915827338129496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.149466192170819</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.269094922737307</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.474893617021277</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.672096908939014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.862576687116564</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$22:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.169352517985612</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.270462633451957</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.463576158940397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.659574468085106</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.999754601226994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.297841726618705</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.429418742586002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.649006622516556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.991489361702128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.999754601226994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$24:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.461151079136691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.601423487544484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.960264900662252</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.999574468085106</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.999877300613497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$25:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.59136690647482</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.830367734282325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999779249448124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.999574468085106</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$26:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.762589928057554</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.972716488730724</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999779249448124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024*2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$27:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.856115107913669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024*4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$28:$G$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.870503597122302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.981020166073547</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024*8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$29:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.877697841726619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97864768683274</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.964679911699779</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024*16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$30:$G$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.884892086330935</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.941874258600237</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024*32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$31:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.902877697841727</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="780291972"/>
+        <c:axId val="200596670"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="780291972"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:crossAx val="200596670"/>
+        <c:delete val="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="200596670"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:crossAx val="780291972"/>
+        <c:delete val="0"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:round/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+    <a:p>
+      <a:pPr algn="l">
+        <a:defRPr sz="1000" b="0" i="0" u="none">
+          <a:latin typeface="함초롬돋움" panose="0"/>
+          <a:ea typeface="함초롬돋움" panose="0"/>
+          <a:cs typeface="함초롬돋움" panose="0"/>
+          <a:sym typeface="함초롬돋움" panose="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr/>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext uri="CC8EB2C9-7E31-499d-B8F2-F6CE61031016">
+      <ho:hncChartStyle xmlns:ho="http://schemas.haansoft.com/office/8.0" layoutIndex="-1" colorIndex="0" styleIndex="0"/>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <c:date1904 val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:p>
+            <a:pPr algn="l">
+              <a:defRPr sz="2000" b="1" i="0" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="함초롬돋움" panose="0"/>
+                <a:ea typeface="함초롬돋움" panose="0"/>
+                <a:cs typeface="함초롬돋움" panose="0"/>
+                <a:sym typeface="함초롬돋움" panose="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="2000" b="1" i="0" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="함초롬돋움" panose="0"/>
+                <a:ea typeface="함초롬돋움" panose="0"/>
+                <a:cs typeface="함초롬돋움" panose="0"/>
+                <a:sym typeface="함초롬돋움" panose="0"/>
+              </a:rPr>
+              <a:t>pps test with kernel launch</a:t>
+            </a:r>
+            <a:endParaRPr/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024*2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024*4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024*8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024*16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024*32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$21:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0915827338129496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.169352517985612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.297841726618705</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.461151079136691</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59136690647482</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.762589928057554</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.856115107913669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.870503597122302</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.877697841726619</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.884892086330935</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.902877697841727</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128 (8.4Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024*2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024*4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024*8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024*16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024*32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$C$21:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.149466192170819</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.270462633451957</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.429418742586002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.601423487544484</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.830367734282325</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.972716488730724</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.981020166073547</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97864768683274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.941874258600237</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256 (4.5Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024*2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024*4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024*8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024*16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024*32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$D$21:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.269094922737307</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.463576158940397</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.649006622516556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.960264900662252</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.999779249448124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.999779249448124</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.964679911699779</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$E$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512 (2.35Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024*2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024*4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024*8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024*16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024*32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$E$21:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.474893617021277</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.659574468085106</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.991489361702128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.999574468085106</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.999574468085106</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$F$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024 (1.2Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024*2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024*4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024*8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024*16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024*32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$F$21:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.672096908939014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1514 (0.8 Mpps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024*2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024*4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024*8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024*16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024*32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$G$21:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.862576687116564</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.999754601226994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999754601226994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.999877300613497</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="780291972"/>
+        <c:axId val="200596670"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="780291972"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:crossAx val="200596670"/>
+        <c:delete val="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="200596670"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:crossAx val="780291972"/>
+        <c:delete val="0"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:round/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr rot="0" vert="horz" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+    <a:p>
+      <a:pPr algn="l">
+        <a:defRPr sz="1000" b="0" i="0" u="none">
+          <a:latin typeface="함초롬돋움" panose="0"/>
+          <a:ea typeface="함초롬돋움" panose="0"/>
+          <a:cs typeface="함초롬돋움" panose="0"/>
+          <a:sym typeface="함초롬돋움" panose="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr/>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext uri="CC8EB2C9-7E31-499d-B8F2-F6CE61031016">
+      <ho:hncChartStyle xmlns:ho="http://schemas.haansoft.com/office/8.0" layoutIndex="-1" colorIndex="0" styleIndex="0"/>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4122,7 +5759,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4239,6 +5876,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="1" fPrintsWithSheet="1"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame fPublished="0">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="차트 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="12592051" cy="6086475"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="1" fPrintsWithSheet="1"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame fPublished="0">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="차트 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="6791325"/>
+        <a:ext cx="12592051" cy="6086475"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4504,8 +6206,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="A1:G52"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="E38" activeCellId="0" sqref="E38:E38"/>
+    <x:sheetView topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="A1" activeCellId="0" sqref="A1:G47"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.550000000000001"/>
@@ -4516,7 +6218,7 @@
   <x:sheetData>
     <x:row r="1" spans="2:7">
       <x:c r="B1" s="7" t="s">
-        <x:v>3</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C1" s="8"/>
       <x:c r="D1" s="8"/>
@@ -4535,22 +6237,22 @@
     <x:row r="3" spans="1:7">
       <x:c r="A3" s="1"/>
       <x:c r="B3" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C3" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E3" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F3" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G3" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
@@ -4693,7 +6395,7 @@
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="A10" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B10" s="1">
         <x:v>13390000</x:v>
@@ -4714,7 +6416,7 @@
     </x:row>
     <x:row r="11" spans="1:7">
       <x:c r="A11" s="1" t="s">
-        <x:v>10</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B11" s="1">
         <x:v>12500000</x:v>
@@ -4733,7 +6435,7 @@
     </x:row>
     <x:row r="12" spans="1:7">
       <x:c r="A12" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B12" s="1">
         <x:v>12550000</x:v>
@@ -4750,7 +6452,7 @@
     </x:row>
     <x:row r="13" spans="1:7">
       <x:c r="A13" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="1">
         <x:v>12480000</x:v>
@@ -4765,7 +6467,7 @@
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="1" t="s">
-        <x:v>15</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="1">
         <x:v>12770000</x:v>
@@ -4778,7 +6480,7 @@
     </x:row>
     <x:row r="18" spans="2:7">
       <x:c r="B18" s="7" t="s">
-        <x:v>21</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C18" s="8"/>
       <x:c r="D18" s="8"/>
@@ -4797,22 +6499,22 @@
     <x:row r="20" spans="1:7">
       <x:c r="A20" s="1"/>
       <x:c r="B20" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C20" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D20" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E20" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F20" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G20" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:7">
@@ -4991,7 +6693,7 @@
     </x:row>
     <x:row r="27" spans="1:7">
       <x:c r="A27" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B27" s="1">
         <x:f t="shared" si="3"/>
@@ -5017,7 +6719,7 @@
     </x:row>
     <x:row r="28" spans="1:7">
       <x:c r="A28" s="1" t="s">
-        <x:v>10</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B28" s="1">
         <x:f t="shared" si="3"/>
@@ -5040,7 +6742,7 @@
     </x:row>
     <x:row r="29" spans="1:7">
       <x:c r="A29" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B29" s="1">
         <x:f t="shared" si="3"/>
@@ -5063,7 +6765,7 @@
     </x:row>
     <x:row r="30" spans="1:7">
       <x:c r="A30" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B30" s="1">
         <x:f t="shared" si="3"/>
@@ -5086,7 +6788,7 @@
     </x:row>
     <x:row r="31" spans="1:7">
       <x:c r="A31" s="1" t="s">
-        <x:v>15</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B31" s="1">
         <x:f t="shared" si="3"/>
@@ -5118,7 +6820,7 @@
     </x:row>
     <x:row r="34" spans="2:7">
       <x:c r="B34" s="7" t="s">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C34" s="8"/>
       <x:c r="D34" s="8"/>
@@ -5137,22 +6839,22 @@
     <x:row r="36" spans="1:7">
       <x:c r="A36" s="1"/>
       <x:c r="B36" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C36" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D36" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E36" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F36" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G36" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:7">
@@ -5168,9 +6870,15 @@
       <x:c r="D37" s="1">
         <x:v>60600</x:v>
       </x:c>
-      <x:c r="E37" s="1"/>
-      <x:c r="F37" s="1"/>
-      <x:c r="G37" s="1"/>
+      <x:c r="E37" s="1">
+        <x:v>60300</x:v>
+      </x:c>
+      <x:c r="F37" s="1">
+        <x:v>37351</x:v>
+      </x:c>
+      <x:c r="G37" s="1">
+        <x:v>25450</x:v>
+      </x:c>
     </x:row>
     <x:row r="38" spans="1:7">
       <x:c r="A38" s="1">
@@ -5185,9 +6893,15 @@
       <x:c r="D38" s="1">
         <x:v>60000</x:v>
       </x:c>
-      <x:c r="E38" s="1"/>
-      <x:c r="F38" s="1"/>
-      <x:c r="G38" s="1"/>
+      <x:c r="E38" s="1">
+        <x:v>36654</x:v>
+      </x:c>
+      <x:c r="F38" s="1">
+        <x:v>18705</x:v>
+      </x:c>
+      <x:c r="G38" s="1">
+        <x:v>12732</x:v>
+      </x:c>
     </x:row>
     <x:row r="39" spans="1:7">
       <x:c r="A39" s="1">
@@ -5202,9 +6916,15 @@
       <x:c r="D39" s="1">
         <x:v>35200</x:v>
       </x:c>
-      <x:c r="E39" s="1"/>
-      <x:c r="F39" s="1"/>
-      <x:c r="G39" s="1"/>
+      <x:c r="E39" s="1">
+        <x:v>18347</x:v>
+      </x:c>
+      <x:c r="F39" s="1">
+        <x:v>9353</x:v>
+      </x:c>
+      <x:c r="G39" s="1">
+        <x:v>6366</x:v>
+      </x:c>
     </x:row>
     <x:row r="40" spans="1:7">
       <x:c r="A40" s="1">
@@ -5219,9 +6939,15 @@
       <x:c r="D40" s="1">
         <x:v>17764</x:v>
       </x:c>
-      <x:c r="E40" s="1"/>
-      <x:c r="F40" s="1"/>
-      <x:c r="G40" s="1"/>
+      <x:c r="E40" s="1">
+        <x:v>9177</x:v>
+      </x:c>
+      <x:c r="F40" s="1">
+        <x:v>4677</x:v>
+      </x:c>
+      <x:c r="G40" s="1">
+        <x:v>3183</x:v>
+      </x:c>
     </x:row>
     <x:row r="41" spans="1:7">
       <x:c r="A41" s="1">
@@ -5236,9 +6962,15 @@
       <x:c r="D41" s="1">
         <x:v>8846</x:v>
       </x:c>
-      <x:c r="E41" s="1"/>
-      <x:c r="F41" s="1"/>
-      <x:c r="G41" s="1"/>
+      <x:c r="E41" s="1">
+        <x:v>4589</x:v>
+      </x:c>
+      <x:c r="F41" s="1">
+        <x:v>2339</x:v>
+      </x:c>
+      <x:c r="G41" s="1">
+        <x:v>1592</x:v>
+      </x:c>
     </x:row>
     <x:row r="42" spans="1:7">
       <x:c r="A42" s="1">
@@ -5253,13 +6985,19 @@
       <x:c r="D42" s="1">
         <x:v>4423</x:v>
       </x:c>
-      <x:c r="E42" s="1"/>
-      <x:c r="F42" s="1"/>
-      <x:c r="G42" s="1"/>
+      <x:c r="E42" s="1">
+        <x:v>2295</x:v>
+      </x:c>
+      <x:c r="F42" s="1">
+        <x:v>1170</x:v>
+      </x:c>
+      <x:c r="G42" s="1">
+        <x:v>796</x:v>
+      </x:c>
     </x:row>
     <x:row r="43" spans="1:7">
       <x:c r="A43" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B43" s="1">
         <x:v>6420</x:v>
@@ -5270,13 +7008,17 @@
       <x:c r="D43" s="1">
         <x:v>2211</x:v>
       </x:c>
-      <x:c r="E43" s="1"/>
-      <x:c r="F43" s="1"/>
+      <x:c r="E43" s="1">
+        <x:v>1147</x:v>
+      </x:c>
+      <x:c r="F43" s="1">
+        <x:v>585</x:v>
+      </x:c>
       <x:c r="G43" s="1"/>
     </x:row>
     <x:row r="44" spans="1:7">
       <x:c r="A44" s="1" t="s">
-        <x:v>10</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B44" s="1">
         <x:v>3050</x:v>
@@ -5287,13 +7029,15 @@
       <x:c r="D44" s="1">
         <x:v>1106</x:v>
       </x:c>
-      <x:c r="E44" s="1"/>
+      <x:c r="E44" s="1">
+        <x:v>574</x:v>
+      </x:c>
       <x:c r="F44" s="1"/>
       <x:c r="G44" s="1"/>
     </x:row>
     <x:row r="45" spans="1:7">
       <x:c r="A45" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B45" s="1">
         <x:v>1532</x:v>
@@ -5310,7 +7054,7 @@
     </x:row>
     <x:row r="46" spans="1:7">
       <x:c r="A46" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B46" s="1">
         <x:v>760</x:v>
@@ -5325,7 +7069,7 @@
     </x:row>
     <x:row r="47" spans="1:7">
       <x:c r="A47" s="1" t="s">
-        <x:v>15</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B47" s="1">
         <x:v>387</x:v>
@@ -5409,22 +7153,22 @@
   <x:sheetData>
     <x:row r="1" spans="2:7" customHeight="1">
       <x:c r="B1" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C1" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D1" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E1" s="10" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C1" s="10" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D1" s="10" t="s">
+      <x:c r="F1" s="10" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="E1" s="10" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F1" s="10" t="s">
-        <x:v>2</x:v>
-      </x:c>
       <x:c r="G1" s="10" t="s">
-        <x:v>1</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="2:13" customHeight="1">
@@ -5581,7 +7325,7 @@
     </x:row>
     <x:row r="9" spans="1:7" customHeight="1">
       <x:c r="A9" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B9" s="4">
         <x:v>2722</x:v>
@@ -5604,7 +7348,7 @@
     </x:row>
     <x:row r="10" spans="1:7" customHeight="1">
       <x:c r="A10" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B10" s="4">
         <x:v>2843</x:v>
@@ -5627,7 +7371,7 @@
     </x:row>
     <x:row r="11" spans="1:7" customHeight="1">
       <x:c r="A11" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B11" s="4">
         <x:v>3133</x:v>
@@ -5650,7 +7394,7 @@
     </x:row>
     <x:row r="12" spans="1:7" customHeight="1">
       <x:c r="A12" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B12" s="4">
         <x:v>3857</x:v>
@@ -5673,7 +7417,7 @@
     </x:row>
     <x:row r="13" spans="1:7" customHeight="1">
       <x:c r="A13" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="B13" s="4">
         <x:v>5125</x:v>
@@ -5696,7 +7440,7 @@
     </x:row>
     <x:row r="14" spans="1:7" customHeight="1">
       <x:c r="A14" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B14" s="4">
         <x:v>7528</x:v>
@@ -5719,7 +7463,7 @@
     </x:row>
     <x:row r="15" spans="1:7" customHeight="1">
       <x:c r="A15" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B15" s="4">
         <x:v>11994</x:v>
@@ -5742,7 +7486,7 @@
     </x:row>
     <x:row r="16" spans="1:7" customHeight="1">
       <x:c r="A16" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B16" s="4">
         <x:v>19883</x:v>
@@ -5765,7 +7509,7 @@
     </x:row>
     <x:row r="17" spans="1:7" customHeight="1">
       <x:c r="A17" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B17" s="4">
         <x:v>37751</x:v>
@@ -5788,7 +7532,7 @@
     </x:row>
     <x:row r="18" spans="1:7" customHeight="1">
       <x:c r="A18" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B18" s="4">
         <x:v>85677</x:v>
@@ -5811,7 +7555,7 @@
     </x:row>
     <x:row r="19" spans="1:7" customHeight="1">
       <x:c r="A19" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B19" s="4">
         <x:v>206878</x:v>
@@ -5925,59 +7669,59 @@
     </x:row>
     <x:row r="48" spans="1:4">
       <x:c r="A48" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B48" s="3"/>
       <x:c r="D48" s="3"/>
     </x:row>
     <x:row r="49" spans="1:1">
       <x:c r="A49" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:1">
       <x:c r="A50" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:1">
       <x:c r="A51" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:1">
       <x:c r="A52" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:1">
       <x:c r="A53" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:1">
       <x:c r="A54" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:1">
       <x:c r="A55" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:1">
       <x:c r="A56" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:1">
       <x:c r="A57" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:1">
       <x:c r="A58" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -6014,7 +7758,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="11" t="s">
-        <x:v>17</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B1" s="9"/>
       <x:c r="C1" s="9"/>
@@ -6030,16 +7774,16 @@
     </x:row>
     <x:row r="3" spans="2:5">
       <x:c r="B3" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C3" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D3" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E3" s="10" t="s">
         <x:v>30</x:v>
-      </x:c>
-      <x:c r="C3" s="10" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D3" s="10" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="E3" s="10" t="s">
-        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5">
@@ -6152,7 +7896,7 @@
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B11" s="4">
         <x:v>7445</x:v>
@@ -6169,7 +7913,7 @@
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="4">
         <x:v>2307</x:v>
@@ -6186,7 +7930,7 @@
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B13" s="4">
         <x:v>3334</x:v>
@@ -6203,7 +7947,7 @@
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="A14" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B14" s="4">
         <x:v>5643</x:v>
@@ -6220,7 +7964,7 @@
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="A15" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="B15" s="4">
         <x:v>8649</x:v>
@@ -6237,7 +7981,7 @@
     </x:row>
     <x:row r="16" spans="1:5">
       <x:c r="A16" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B16" s="4">
         <x:v>7925</x:v>
@@ -6254,7 +7998,7 @@
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="A17" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B17" s="4">
         <x:v>19881</x:v>
@@ -6271,7 +8015,7 @@
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="A18" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B18" s="4">
         <x:v>26627</x:v>
@@ -6288,7 +8032,7 @@
     </x:row>
     <x:row r="19" spans="1:5">
       <x:c r="A19" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B19" s="4">
         <x:v>40525</x:v>
@@ -6305,7 +8049,7 @@
     </x:row>
     <x:row r="20" spans="1:5">
       <x:c r="A20" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B20" s="4">
         <x:v>74741</x:v>
@@ -6322,7 +8066,7 @@
     </x:row>
     <x:row r="21" spans="1:5">
       <x:c r="A21" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B21" s="4">
         <x:v>150490</x:v>
@@ -6339,7 +8083,7 @@
     </x:row>
     <x:row r="25" spans="1:5" ht="24.949999999999999" customHeight="1">
       <x:c r="A25" s="11" t="s">
-        <x:v>17</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B25" s="9"/>
       <x:c r="C25" s="9"/>
@@ -6355,10 +8099,10 @@
     </x:row>
     <x:row r="27" spans="2:3">
       <x:c r="B27" s="10" t="s">
-        <x:v>2</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C27" s="10" t="s">
-        <x:v>1</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="2:3">
@@ -6433,7 +8177,7 @@
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B35">
         <x:v>1704662</x:v>
@@ -6444,7 +8188,7 @@
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B36">
         <x:v>888145</x:v>
@@ -6455,7 +8199,7 @@
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="A37" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B37">
         <x:v>501401</x:v>
@@ -6466,7 +8210,7 @@
     </x:row>
     <x:row r="38" spans="1:3">
       <x:c r="A38" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B38">
         <x:v>332799</x:v>
@@ -6477,7 +8221,7 @@
     </x:row>
     <x:row r="39" spans="1:3">
       <x:c r="A39" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="B39">
         <x:v>234809</x:v>
@@ -6488,7 +8232,7 @@
     </x:row>
     <x:row r="40" spans="1:3">
       <x:c r="A40" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B40">
         <x:v>185326</x:v>
@@ -6499,7 +8243,7 @@
     </x:row>
     <x:row r="41" spans="1:3">
       <x:c r="A41" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B41">
         <x:v>161905</x:v>
@@ -6510,7 +8254,7 @@
     </x:row>
     <x:row r="42" spans="1:3">
       <x:c r="A42" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B42">
         <x:v>150163</x:v>
@@ -6521,7 +8265,7 @@
     </x:row>
     <x:row r="43" spans="1:3">
       <x:c r="A43" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B43">
         <x:v>145611</x:v>
@@ -6532,7 +8276,7 @@
     </x:row>
     <x:row r="44" spans="1:3">
       <x:c r="A44" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B44">
         <x:v>148653</x:v>
@@ -6543,7 +8287,7 @@
     </x:row>
     <x:row r="45" spans="1:3">
       <x:c r="A45" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B45">
         <x:v>167357</x:v>
@@ -6554,7 +8298,7 @@
     </x:row>
     <x:row r="48" spans="1:7" ht="24.949999999999999" customHeight="1">
       <x:c r="A48" s="11" t="s">
-        <x:v>28</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B48" s="7"/>
       <x:c r="C48" s="7"/>
@@ -6574,16 +8318,16 @@
     </x:row>
     <x:row r="50" spans="2:5">
       <x:c r="B50" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C50" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D50" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E50" s="10" t="s">
         <x:v>30</x:v>
-      </x:c>
-      <x:c r="C50" s="10" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D50" s="10" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="E50" s="10" t="s">
-        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="2:5">
@@ -6696,7 +8440,7 @@
     </x:row>
     <x:row r="58" spans="1:5">
       <x:c r="A58" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B58" s="4">
         <x:v>2330</x:v>
@@ -6713,7 +8457,7 @@
     </x:row>
     <x:row r="59" spans="1:5">
       <x:c r="A59" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B59" s="4">
         <x:v>3582</x:v>
@@ -6730,7 +8474,7 @@
     </x:row>
     <x:row r="60" spans="1:5">
       <x:c r="A60" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B60" s="4">
         <x:v>3213</x:v>
@@ -6747,7 +8491,7 @@
     </x:row>
     <x:row r="61" spans="1:5">
       <x:c r="A61" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B61" s="4">
         <x:v>3588</x:v>
@@ -6764,7 +8508,7 @@
     </x:row>
     <x:row r="62" spans="1:5">
       <x:c r="A62" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="B62" s="5">
         <x:v>12283</x:v>
@@ -6781,7 +8525,7 @@
     </x:row>
     <x:row r="63" spans="1:5">
       <x:c r="A63" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B63" s="4">
         <x:v>7954</x:v>
@@ -6798,7 +8542,7 @@
     </x:row>
     <x:row r="64" spans="1:5">
       <x:c r="A64" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B64" s="4">
         <x:v>11599</x:v>
@@ -6815,7 +8559,7 @@
     </x:row>
     <x:row r="65" spans="1:5">
       <x:c r="A65" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B65" s="4">
         <x:v>20553</x:v>
@@ -6832,7 +8576,7 @@
     </x:row>
     <x:row r="66" spans="1:5">
       <x:c r="A66" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B66" s="4">
         <x:v>38486</x:v>
@@ -6849,7 +8593,7 @@
     </x:row>
     <x:row r="67" spans="1:5">
       <x:c r="A67" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B67" s="4">
         <x:v>75167</x:v>
@@ -6866,7 +8610,7 @@
     </x:row>
     <x:row r="68" spans="1:5">
       <x:c r="A68" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B68" s="4">
         <x:v>161317</x:v>
@@ -6883,7 +8627,7 @@
     </x:row>
     <x:row r="73" spans="1:5" ht="24.949999999999999" customHeight="1">
       <x:c r="A73" s="11" t="s">
-        <x:v>28</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B73" s="7"/>
       <x:c r="C73" s="7"/>
@@ -6899,10 +8643,10 @@
     </x:row>
     <x:row r="75" spans="2:3">
       <x:c r="B75" s="10" t="s">
-        <x:v>2</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C75" s="10" t="s">
-        <x:v>1</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="2:3">
@@ -6977,7 +8721,7 @@
     </x:row>
     <x:row r="83" spans="1:3">
       <x:c r="A83" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B83">
         <x:v>1708597</x:v>
@@ -6988,7 +8732,7 @@
     </x:row>
     <x:row r="84" spans="1:3">
       <x:c r="A84" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B84">
         <x:v>889942</x:v>
@@ -6999,7 +8743,7 @@
     </x:row>
     <x:row r="85" spans="1:3">
       <x:c r="A85" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B85">
         <x:v>506309</x:v>
@@ -7010,7 +8754,7 @@
     </x:row>
     <x:row r="86" spans="1:3">
       <x:c r="A86" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B86">
         <x:v>344510</x:v>
@@ -7021,7 +8765,7 @@
     </x:row>
     <x:row r="87" spans="1:3">
       <x:c r="A87" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="B87">
         <x:v>242647</x:v>
@@ -7032,7 +8776,7 @@
     </x:row>
     <x:row r="88" spans="1:3">
       <x:c r="A88" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B88">
         <x:v>185274</x:v>
@@ -7043,7 +8787,7 @@
     </x:row>
     <x:row r="89" spans="1:3">
       <x:c r="A89" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B89">
         <x:v>158391</x:v>
@@ -7054,7 +8798,7 @@
     </x:row>
     <x:row r="90" spans="1:3">
       <x:c r="A90" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B90">
         <x:v>149039</x:v>
@@ -7065,7 +8809,7 @@
     </x:row>
     <x:row r="91" spans="1:3">
       <x:c r="A91" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B91">
         <x:v>153874</x:v>
@@ -7076,7 +8820,7 @@
     </x:row>
     <x:row r="92" spans="1:3">
       <x:c r="A92" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B92">
         <x:v>154735</x:v>
@@ -7087,7 +8831,7 @@
     </x:row>
     <x:row r="93" spans="1:3">
       <x:c r="A93" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B93">
         <x:v>169481</x:v>
@@ -7135,4 +8879,938 @@
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <x:drawing r:id="rId1"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr codeName="Sheet5"/>
+  <x:dimension ref="A1:G47"/>
+  <x:sheetViews>
+    <x:sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="H16" activeCellId="0" sqref="H16:H16"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.550000000000001"/>
+  <x:cols>
+    <x:col min="1" max="1" width="13.19921875" customWidth="1"/>
+    <x:col min="2" max="7" width="22.4453125" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="2:7">
+      <x:c r="B1" s="7" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C1" s="8"/>
+      <x:c r="D1" s="8"/>
+      <x:c r="E1" s="8"/>
+      <x:c r="F1" s="8"/>
+      <x:c r="G1" s="8"/>
+    </x:row>
+    <x:row r="2" spans="2:7">
+      <x:c r="B2" s="8"/>
+      <x:c r="C2" s="8"/>
+      <x:c r="D2" s="8"/>
+      <x:c r="E2" s="8"/>
+      <x:c r="F2" s="8"/>
+      <x:c r="G2" s="8"/>
+    </x:row>
+    <x:row r="3" spans="1:7">
+      <x:c r="A3" s="1"/>
+      <x:c r="B3" s="1" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C3" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D3" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E3" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F3" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G3" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="A4" s="1">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B4">
+        <x:v>1273000</x:v>
+      </x:c>
+      <x:c r="C4" s="1">
+        <x:v>1260000</x:v>
+      </x:c>
+      <x:c r="D4" s="1">
+        <x:v>1219000</x:v>
+      </x:c>
+      <x:c r="E4" s="1">
+        <x:v>1116000</x:v>
+      </x:c>
+      <x:c r="F4" s="1">
+        <x:v>804500</x:v>
+      </x:c>
+      <x:c r="G4" s="1">
+        <x:v>703000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:7">
+      <x:c r="A5" s="1">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B5" s="1">
+        <x:v>2354000</x:v>
+      </x:c>
+      <x:c r="C5" s="1">
+        <x:v>2280000</x:v>
+      </x:c>
+      <x:c r="D5" s="1">
+        <x:v>2100000</x:v>
+      </x:c>
+      <x:c r="E5" s="1">
+        <x:v>1550000</x:v>
+      </x:c>
+      <x:c r="F5" s="1">
+        <x:v>1197000</x:v>
+      </x:c>
+      <x:c r="G5" s="1">
+        <x:v>814800</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:7">
+      <x:c r="A6" s="1">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B6" s="1">
+        <x:v>4140000</x:v>
+      </x:c>
+      <x:c r="C6" s="1">
+        <x:v>3620000</x:v>
+      </x:c>
+      <x:c r="D6" s="1">
+        <x:v>2940000</x:v>
+      </x:c>
+      <x:c r="E6" s="1">
+        <x:v>2330000</x:v>
+      </x:c>
+      <x:c r="F6" s="1">
+        <x:v>1197000</x:v>
+      </x:c>
+      <x:c r="G6" s="1">
+        <x:v>814800</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:7">
+      <x:c r="A7" s="1">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="B7" s="1">
+        <x:v>6410000</x:v>
+      </x:c>
+      <x:c r="C7" s="1">
+        <x:v>5070000</x:v>
+      </x:c>
+      <x:c r="D7" s="1">
+        <x:v>4350000</x:v>
+      </x:c>
+      <x:c r="E7" s="1">
+        <x:v>2349000</x:v>
+      </x:c>
+      <x:c r="F7" s="1">
+        <x:v>1197000</x:v>
+      </x:c>
+      <x:c r="G7" s="1">
+        <x:v>814900</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:7">
+      <x:c r="A8" s="1">
+        <x:v>512</x:v>
+      </x:c>
+      <x:c r="B8" s="1">
+        <x:v>8220000</x:v>
+      </x:c>
+      <x:c r="C8" s="1">
+        <x:v>7000000</x:v>
+      </x:c>
+      <x:c r="D8" s="1">
+        <x:v>4529000</x:v>
+      </x:c>
+      <x:c r="E8" s="1">
+        <x:v>2349000</x:v>
+      </x:c>
+      <x:c r="F8" s="1">
+        <x:v>1197000</x:v>
+      </x:c>
+      <x:c r="G8" s="1">
+        <x:v>815000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:7">
+      <x:c r="A9" s="1">
+        <x:v>1024</x:v>
+      </x:c>
+      <x:c r="B9" s="1">
+        <x:v>10600000</x:v>
+      </x:c>
+      <x:c r="C9" s="1">
+        <x:v>8200000</x:v>
+      </x:c>
+      <x:c r="D9" s="1">
+        <x:v>4529000</x:v>
+      </x:c>
+      <x:c r="E9" s="1">
+        <x:v>2350000</x:v>
+      </x:c>
+      <x:c r="F9" s="1">
+        <x:v>1197000</x:v>
+      </x:c>
+      <x:c r="G9" s="1">
+        <x:v>815000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:7">
+      <x:c r="A10" s="1" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B10" s="1">
+        <x:v>11900000</x:v>
+      </x:c>
+      <x:c r="C10" s="1">
+        <x:v>8430000</x:v>
+      </x:c>
+      <x:c r="D10" s="1">
+        <x:v>4530000</x:v>
+      </x:c>
+      <x:c r="E10" s="1">
+        <x:v>2350000</x:v>
+      </x:c>
+      <x:c r="F10" s="1">
+        <x:v>1197000</x:v>
+      </x:c>
+      <x:c r="G10" s="1"/>
+    </x:row>
+    <x:row r="11" spans="1:7">
+      <x:c r="A11" s="1" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B11" s="1">
+        <x:v>12100000</x:v>
+      </x:c>
+      <x:c r="C11" s="1">
+        <x:v>8270000</x:v>
+      </x:c>
+      <x:c r="D11" s="1">
+        <x:v>4530000</x:v>
+      </x:c>
+      <x:c r="E11" s="1">
+        <x:v>2350000</x:v>
+      </x:c>
+      <x:c r="F11" s="1"/>
+      <x:c r="G11" s="1"/>
+    </x:row>
+    <x:row r="12" spans="1:7">
+      <x:c r="A12" s="1" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B12" s="1">
+        <x:v>12200000</x:v>
+      </x:c>
+      <x:c r="C12" s="1">
+        <x:v>8250000</x:v>
+      </x:c>
+      <x:c r="D12" s="1">
+        <x:v>4370000</x:v>
+      </x:c>
+      <x:c r="E12" s="1"/>
+      <x:c r="F12" s="1"/>
+      <x:c r="G12" s="1"/>
+    </x:row>
+    <x:row r="13" spans="1:7">
+      <x:c r="A13" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B13" s="1">
+        <x:v>12300000</x:v>
+      </x:c>
+      <x:c r="C13" s="1">
+        <x:v>7940000</x:v>
+      </x:c>
+      <x:c r="D13" s="1"/>
+      <x:c r="E13" s="1"/>
+      <x:c r="F13" s="1"/>
+      <x:c r="G13" s="1"/>
+    </x:row>
+    <x:row r="14" spans="1:7">
+      <x:c r="A14" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B14" s="1">
+        <x:v>12550000</x:v>
+      </x:c>
+      <x:c r="C14" s="1"/>
+      <x:c r="D14" s="1"/>
+      <x:c r="E14" s="1"/>
+      <x:c r="F14" s="1"/>
+      <x:c r="G14" s="1"/>
+    </x:row>
+    <x:row r="18" spans="2:7">
+      <x:c r="B18" s="7" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C18" s="8"/>
+      <x:c r="D18" s="8"/>
+      <x:c r="E18" s="8"/>
+      <x:c r="F18" s="8"/>
+      <x:c r="G18" s="8"/>
+    </x:row>
+    <x:row r="19" spans="2:7">
+      <x:c r="B19" s="8"/>
+      <x:c r="C19" s="8"/>
+      <x:c r="D19" s="8"/>
+      <x:c r="E19" s="8"/>
+      <x:c r="F19" s="8"/>
+      <x:c r="G19" s="8"/>
+    </x:row>
+    <x:row r="20" spans="1:7">
+      <x:c r="A20" s="1"/>
+      <x:c r="B20" s="1" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C20" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D20" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E20" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F20" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G20" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:7">
+      <x:c r="A21" s="1">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B21" s="1">
+        <x:f>B4/13900000</x:f>
+        <x:v>0.091582733812949638</x:v>
+      </x:c>
+      <x:c r="C21">
+        <x:f>C4/MAX($C$4:$C$13)</x:f>
+        <x:v>0.1494661921708185</x:v>
+      </x:c>
+      <x:c r="D21">
+        <x:f>D4/MAX($D$4:$D$13)</x:f>
+        <x:v>0.26909492273730684</x:v>
+      </x:c>
+      <x:c r="E21">
+        <x:f>E4/MAX($E$4:$E$13)</x:f>
+        <x:v>0.47489361702127658</x:v>
+      </x:c>
+      <x:c r="F21">
+        <x:f>F4/MAX($F$4:$F$13)</x:f>
+        <x:v>0.67209690893901419</x:v>
+      </x:c>
+      <x:c r="G21">
+        <x:f>G4/MAX($G$4:$G$13)</x:f>
+        <x:v>0.86257668711656443</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:7">
+      <x:c r="A22" s="1">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B22" s="1">
+        <x:f t="shared" ref="B22:B31" si="0">B5/13900000</x:f>
+        <x:v>0.16935251798561152</x:v>
+      </x:c>
+      <x:c r="C22">
+        <x:f t="shared" ref="C22:C31" si="1">C5/MAX($C$4:$C$13)</x:f>
+        <x:v>0.27046263345195731</x:v>
+      </x:c>
+      <x:c r="D22">
+        <x:f t="shared" ref="D22:D31" si="2">D5/MAX($D$4:$D$13)</x:f>
+        <x:v>0.46357615894039733</x:v>
+      </x:c>
+      <x:c r="E22">
+        <x:f t="shared" ref="E22:E31" si="3">E5/MAX($E$4:$E$13)</x:f>
+        <x:v>0.65957446808510634</x:v>
+      </x:c>
+      <x:c r="F22">
+        <x:f t="shared" ref="F22:F31" si="4">F5/MAX($F$4:$F$13)</x:f>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G22">
+        <x:f t="shared" ref="G22:G31" si="5">G5/MAX($G$4:$G$13)</x:f>
+        <x:v>0.99975460122699389</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:7">
+      <x:c r="A23" s="1">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B23" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.29784172661870506</x:v>
+      </x:c>
+      <x:c r="C23">
+        <x:f t="shared" si="1"/>
+        <x:v>0.42941874258600238</x:v>
+      </x:c>
+      <x:c r="D23">
+        <x:f t="shared" si="2"/>
+        <x:v>0.64900662251655628</x:v>
+      </x:c>
+      <x:c r="E23">
+        <x:f t="shared" si="3"/>
+        <x:v>0.99148936170212765</x:v>
+      </x:c>
+      <x:c r="F23">
+        <x:f t="shared" si="4"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G23">
+        <x:f t="shared" si="5"/>
+        <x:v>0.99975460122699389</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:7">
+      <x:c r="A24" s="1">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="B24" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.46115107913669062</x:v>
+      </x:c>
+      <x:c r="C24">
+        <x:f t="shared" si="1"/>
+        <x:v>0.60142348754448394</x:v>
+      </x:c>
+      <x:c r="D24">
+        <x:f t="shared" si="2"/>
+        <x:v>0.96026490066225167</x:v>
+      </x:c>
+      <x:c r="E24">
+        <x:f t="shared" si="3"/>
+        <x:v>0.99957446808510642</x:v>
+      </x:c>
+      <x:c r="F24">
+        <x:f t="shared" si="4"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G24">
+        <x:f t="shared" si="5"/>
+        <x:v>0.99987730061349689</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:7">
+      <x:c r="A25" s="1">
+        <x:v>512</x:v>
+      </x:c>
+      <x:c r="B25" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.59136690647482015</x:v>
+      </x:c>
+      <x:c r="C25">
+        <x:f t="shared" si="1"/>
+        <x:v>0.83036773428232502</x:v>
+      </x:c>
+      <x:c r="D25">
+        <x:f t="shared" si="2"/>
+        <x:v>0.99977924944812357</x:v>
+      </x:c>
+      <x:c r="E25">
+        <x:f t="shared" si="3"/>
+        <x:v>0.99957446808510642</x:v>
+      </x:c>
+      <x:c r="F25">
+        <x:f t="shared" si="4"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G25">
+        <x:f t="shared" si="5"/>
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:7">
+      <x:c r="A26" s="1">
+        <x:v>1024</x:v>
+      </x:c>
+      <x:c r="B26" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.76258992805755399</x:v>
+      </x:c>
+      <x:c r="C26">
+        <x:f t="shared" si="1"/>
+        <x:v>0.97271648873072358</x:v>
+      </x:c>
+      <x:c r="D26">
+        <x:f t="shared" si="2"/>
+        <x:v>0.99977924944812357</x:v>
+      </x:c>
+      <x:c r="E26">
+        <x:f t="shared" si="3"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F26">
+        <x:f t="shared" si="4"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G26">
+        <x:f t="shared" si="5"/>
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:7">
+      <x:c r="A27" s="1" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B27" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.85611510791366907</x:v>
+      </x:c>
+      <x:c r="C27">
+        <x:f t="shared" si="1"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D27">
+        <x:f t="shared" si="2"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E27">
+        <x:f t="shared" si="3"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F27">
+        <x:f t="shared" si="4"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G27">
+        <x:f t="shared" si="5"/>
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:7">
+      <x:c r="A28" s="1" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B28" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.87050359712230219</x:v>
+      </x:c>
+      <x:c r="C28">
+        <x:f t="shared" si="1"/>
+        <x:v>0.98102016607354681</x:v>
+      </x:c>
+      <x:c r="D28">
+        <x:f t="shared" si="2"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E28">
+        <x:f t="shared" si="3"/>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F28">
+        <x:f t="shared" si="4"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G28">
+        <x:f t="shared" si="5"/>
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:7">
+      <x:c r="A29" s="1" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B29" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.87769784172661869</x:v>
+      </x:c>
+      <x:c r="C29">
+        <x:f t="shared" si="1"/>
+        <x:v>0.97864768683274017</x:v>
+      </x:c>
+      <x:c r="D29">
+        <x:f t="shared" si="2"/>
+        <x:v>0.96467991169977929</x:v>
+      </x:c>
+      <x:c r="E29">
+        <x:f t="shared" si="3"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F29">
+        <x:f t="shared" si="4"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G29">
+        <x:f t="shared" si="5"/>
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:7">
+      <x:c r="A30" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B30" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.8848920863309353</x:v>
+      </x:c>
+      <x:c r="C30">
+        <x:f t="shared" si="1"/>
+        <x:v>0.94187425860023721</x:v>
+      </x:c>
+      <x:c r="D30">
+        <x:f t="shared" si="2"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E30">
+        <x:f t="shared" si="3"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F30">
+        <x:f t="shared" si="4"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G30">
+        <x:f t="shared" si="5"/>
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:7">
+      <x:c r="A31" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B31" s="1">
+        <x:f t="shared" si="0"/>
+        <x:v>0.90287769784172667</x:v>
+      </x:c>
+      <x:c r="C31">
+        <x:f t="shared" si="1"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="D31">
+        <x:f t="shared" si="2"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E31">
+        <x:f t="shared" si="3"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F31">
+        <x:f t="shared" si="4"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G31">
+        <x:f t="shared" si="5"/>
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:7">
+      <x:c r="A33" s="1"/>
+      <x:c r="B33" s="1"/>
+      <x:c r="C33" s="1"/>
+      <x:c r="D33" s="1"/>
+      <x:c r="E33" s="1"/>
+      <x:c r="F33" s="1"/>
+      <x:c r="G33" s="1"/>
+    </x:row>
+    <x:row r="34" spans="2:7">
+      <x:c r="B34" s="7" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C34" s="8"/>
+      <x:c r="D34" s="8"/>
+      <x:c r="E34" s="8"/>
+      <x:c r="F34" s="8"/>
+      <x:c r="G34" s="8"/>
+    </x:row>
+    <x:row r="35" spans="2:7">
+      <x:c r="B35" s="8"/>
+      <x:c r="C35" s="8"/>
+      <x:c r="D35" s="8"/>
+      <x:c r="E35" s="8"/>
+      <x:c r="F35" s="8"/>
+      <x:c r="G35" s="8"/>
+    </x:row>
+    <x:row r="36" spans="1:7">
+      <x:c r="A36" s="1"/>
+      <x:c r="B36" s="1" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C36" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D36" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E36" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F36" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G36" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:7">
+      <x:c r="A37" s="1">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B37">
+        <x:v>39530</x:v>
+      </x:c>
+      <x:c r="C37" s="1">
+        <x:v>39470</x:v>
+      </x:c>
+      <x:c r="D37" s="1">
+        <x:v>38000</x:v>
+      </x:c>
+      <x:c r="E37" s="1">
+        <x:v>34000</x:v>
+      </x:c>
+      <x:c r="F37" s="1">
+        <x:v>25100</x:v>
+      </x:c>
+      <x:c r="G37" s="1">
+        <x:v>21970</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:7">
+      <x:c r="A38" s="1">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B38" s="1">
+        <x:v>36500</x:v>
+      </x:c>
+      <x:c r="C38" s="1">
+        <x:v>35600</x:v>
+      </x:c>
+      <x:c r="D38" s="1">
+        <x:v>32900</x:v>
+      </x:c>
+      <x:c r="E38" s="1">
+        <x:v>24270</x:v>
+      </x:c>
+      <x:c r="F38" s="1">
+        <x:v>18600</x:v>
+      </x:c>
+      <x:c r="G38" s="1">
+        <x:v>12700</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:7">
+      <x:c r="A39" s="1">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B39" s="1">
+        <x:v>31900</x:v>
+      </x:c>
+      <x:c r="C39" s="1">
+        <x:v>28400</x:v>
+      </x:c>
+      <x:c r="D39" s="1">
+        <x:v>22900</x:v>
+      </x:c>
+      <x:c r="E39" s="1">
+        <x:v>18200</x:v>
+      </x:c>
+      <x:c r="F39" s="1">
+        <x:v>9347</x:v>
+      </x:c>
+      <x:c r="G39" s="1">
+        <x:v>6363</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:7">
+      <x:c r="A40" s="1">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="B40" s="1">
+        <x:v>25133</x:v>
+      </x:c>
+      <x:c r="C40" s="1">
+        <x:v>19800</x:v>
+      </x:c>
+      <x:c r="D40" s="1">
+        <x:v>17000</x:v>
+      </x:c>
+      <x:c r="E40" s="1">
+        <x:v>9170</x:v>
+      </x:c>
+      <x:c r="F40" s="1">
+        <x:v>4676</x:v>
+      </x:c>
+      <x:c r="G40" s="1">
+        <x:v>3183</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:7">
+      <x:c r="A41" s="1">
+        <x:v>512</x:v>
+      </x:c>
+      <x:c r="B41" s="1">
+        <x:v>16000</x:v>
+      </x:c>
+      <x:c r="C41" s="1">
+        <x:v>13600</x:v>
+      </x:c>
+      <x:c r="D41" s="1">
+        <x:v>8846</x:v>
+      </x:c>
+      <x:c r="E41" s="1">
+        <x:v>4589</x:v>
+      </x:c>
+      <x:c r="F41" s="1">
+        <x:v>2339</x:v>
+      </x:c>
+      <x:c r="G41" s="1">
+        <x:v>1592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:7">
+      <x:c r="A42" s="1">
+        <x:v>1024</x:v>
+      </x:c>
+      <x:c r="B42" s="1">
+        <x:v>10425</x:v>
+      </x:c>
+      <x:c r="C42" s="1">
+        <x:v>8020</x:v>
+      </x:c>
+      <x:c r="D42" s="1">
+        <x:v>4423</x:v>
+      </x:c>
+      <x:c r="E42" s="1">
+        <x:v>2295</x:v>
+      </x:c>
+      <x:c r="F42" s="1">
+        <x:v>1169</x:v>
+      </x:c>
+      <x:c r="G42" s="1">
+        <x:v>796</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:7">
+      <x:c r="A43" s="1" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B43" s="1">
+        <x:v>5830</x:v>
+      </x:c>
+      <x:c r="C43" s="1">
+        <x:v>4113</x:v>
+      </x:c>
+      <x:c r="D43" s="1">
+        <x:v>2211</x:v>
+      </x:c>
+      <x:c r="E43" s="1">
+        <x:v>1147</x:v>
+      </x:c>
+      <x:c r="F43" s="1">
+        <x:v>585</x:v>
+      </x:c>
+      <x:c r="G43" s="1"/>
+    </x:row>
+    <x:row r="44" spans="1:7">
+      <x:c r="A44" s="1" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B44" s="1">
+        <x:v>2960</x:v>
+      </x:c>
+      <x:c r="C44" s="1">
+        <x:v>2020</x:v>
+      </x:c>
+      <x:c r="D44" s="1">
+        <x:v>1106</x:v>
+      </x:c>
+      <x:c r="E44" s="1">
+        <x:v>574</x:v>
+      </x:c>
+      <x:c r="F44" s="1"/>
+      <x:c r="G44" s="1"/>
+    </x:row>
+    <x:row r="45" spans="1:7">
+      <x:c r="A45" s="1" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B45" s="1">
+        <x:v>1490</x:v>
+      </x:c>
+      <x:c r="C45" s="1">
+        <x:v>1008</x:v>
+      </x:c>
+      <x:c r="D45" s="1">
+        <x:v>533</x:v>
+      </x:c>
+      <x:c r="E45" s="1"/>
+      <x:c r="F45" s="1"/>
+      <x:c r="G45" s="1"/>
+    </x:row>
+    <x:row r="46" spans="1:7">
+      <x:c r="A46" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B46" s="1">
+        <x:v>752</x:v>
+      </x:c>
+      <x:c r="C46" s="1">
+        <x:v>485</x:v>
+      </x:c>
+      <x:c r="D46" s="1"/>
+      <x:c r="E46" s="1"/>
+      <x:c r="F46" s="1"/>
+      <x:c r="G46" s="1"/>
+    </x:row>
+    <x:row r="47" spans="1:7">
+      <x:c r="A47" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B47" s="1">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="C47" s="1"/>
+      <x:c r="D47" s="1"/>
+      <x:c r="E47" s="1"/>
+      <x:c r="F47" s="1"/>
+      <x:c r="G47" s="1"/>
+    </x:row>
+  </x:sheetData>
+  <x:mergeCells count="3">
+    <x:mergeCell ref="B1:G2"/>
+    <x:mergeCell ref="B18:G19"/>
+    <x:mergeCell ref="B34:G35"/>
+  </x:mergeCells>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr codeName="Sheet6"/>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="P61" activeCellId="0" sqref="P61:P61"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.550000000000001"/>
+  <x:sheetData/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <x:drawing r:id="rId1"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
03.02 additional test markdown update
</commit_message>
<xml_diff>
--- a/batch_size_test.xlsx
+++ b/batch_size_test.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.5152"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="18168" windowHeight="8664" tabRatio="626" activeTab="5"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="22788" windowHeight="8664" tabRatio="517" activeTab="4"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="02.25 persistent loop" sheetId="1" r:id="rId4"/>
@@ -19,7 +19,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="33">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="38">
+  <x:si>
+    <x:t>1024*256</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1024 (1.2Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 * 1024 * 32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 * 1024 * 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>256 (4.5Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 * 1024 * 8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 * 1024 * 16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ascending Order</x:t>
+  </x:si>
+  <x:si>
+    <x:t>512 (2.35Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 * 1024 * 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>128 (8.4Mpps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1514 (0.8 Mpps)</x:t>
+  </x:si>
   <x:si>
     <x:t>64 * 1024</x:t>
   </x:si>
@@ -33,43 +69,7 @@
     <x:t>64 * 128</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 1024 * 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>256 (4.5Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ascending Order</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64 * 1024 * 8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64 * 1024 * 32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>512 (2.35Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>128 (8.4Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64 * 1024 * 16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1024 (1.2Mpps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64 * 1024 * 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1514 (0.8 Mpps)</x:t>
-  </x:si>
-  <x:si>
     <x:t>packet size별 batch size에 따른 cudaMemcpy call 횟수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>once / random data</x:t>
   </x:si>
   <x:si>
     <x:t>64 (13.8~14.0Mpps)</x:t>
@@ -78,7 +78,16 @@
     <x:t>once / normal data</x:t>
   </x:si>
   <x:si>
+    <x:t>once / random data</x:t>
+  </x:si>
+  <x:si>
     <x:t>Descending Order</x:t>
+  </x:si>
+  <x:si>
+    <x:t>packet size별 batch size에 따른 rx rate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100times loop / random data</x:t>
   </x:si>
   <x:si>
     <x:t>1024*2</x:t>
@@ -87,37 +96,43 @@
     <x:t>1024*4</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 64</x:t>
+    <x:t>1024*32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64 * 32</x:t>
   </x:si>
   <x:si>
     <x:t>1024*8</x:t>
   </x:si>
   <x:si>
+    <x:t>64 * 64</x:t>
+  </x:si>
+  <x:si>
     <x:t>1024*16</x:t>
   </x:si>
   <x:si>
-    <x:t>64 * 32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1024*32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100times loop / random data</x:t>
-  </x:si>
-  <x:si>
-    <x:t>packet size별 batch size에 따른 rx rate</x:t>
+    <x:t>100 times loop / normal data</x:t>
   </x:si>
   <x:si>
     <x:t>same size loop / normal data</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100 times loop / normal data</x:t>
   </x:si>
   <x:si>
     <x:t>same size loop / random data</x:t>
   </x:si>
   <x:si>
     <x:t>packet size별 batch size에 따른 pps</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1024*512</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1024*128</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1024*64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ㄴㄴㄴㄴ</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -267,7 +282,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="12">
+  <x:cellXfs count="14">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -354,6 +369,22 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="right" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="right" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="6">
     <x:cellStyle xfId="15" builtinId="5" iLevel="0"/>
@@ -369,6 +400,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -451,6 +483,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -485,6 +518,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -529,6 +563,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -572,6 +607,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -655,8 +691,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
-            <x:color indexed="64"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -667,7 +703,6 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
-            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
         </x:dxf>
@@ -677,8 +712,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
-            <x:color indexed="64"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -694,7 +729,6 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
-            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
           <x:border>
@@ -709,8 +743,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
-            <x:color indexed="64"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -726,7 +760,6 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
-            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
           <x:border>
@@ -764,7 +797,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1428,7 +1461,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1812,7 +1845,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2515,7 +2548,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2936,7 +2969,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3639,7 +3672,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -4060,7 +4093,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -4120,11 +4153,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$21</c:f>
+              <c:f>'02.28 kernel launch'!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4132,54 +4165,55 @@
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$21:$G$21</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0915827338129496</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.149466192170819</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.269094922737307</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.474893617021277</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.672096908939014</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.862576687116564</c:v>
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4190,11 +4224,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$22</c:f>
+              <c:f>'02.28 kernel launch'!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4202,54 +4236,55 @@
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$22:$G$22</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.169352517985612</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.270462633451957</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.463576158940397</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.659574468085106</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.999754601226994</c:v>
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$21:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4260,11 +4295,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$23</c:f>
+              <c:f>'02.28 kernel launch'!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4272,54 +4307,55 @@
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$23:$G$23</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.297841726618705</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.429418742586002</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.649006622516556</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.991489361702128</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.999754601226994</c:v>
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$22:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4330,11 +4366,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$24</c:f>
+              <c:f>'02.28 kernel launch'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>256</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4342,54 +4378,55 @@
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$24:$G$24</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.461151079136691</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.601423487544484</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.960264900662252</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.999574468085106</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.999877300613497</c:v>
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4398,68 +4435,58 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>512</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$25:$G$25</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.59136690647482</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.830367734282325</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.999779249448124</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.999574468085106</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$24:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0915827338129496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.149466192170819</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.269094922737307</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.474893617021277</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.672096908939014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.862576687116564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4468,68 +4495,58 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1024</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$26:$G$26</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.762589928057554</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.972716488730724</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.999779249448124</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$25:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.169352517985612</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.270462633451957</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.463576158940397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.659574468085106</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.999754601226994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4538,68 +4555,58 @@
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1024*2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$27:$G$27</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.856115107913669</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$26:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.297841726618705</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.429418742586002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.649006622516556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.991489361702128</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.999754601226994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4608,68 +4615,58 @@
         <c:ser>
           <c:idx val="7"/>
           <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$28</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1024*4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$28:$G$28</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.870503597122302</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.981020166073547</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'02.28 kernel launch'!$B$27:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.461151079136691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.601423487544484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.960264900662252</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.999574468085106</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.999877300613497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4678,208 +4675,58 @@
         <c:ser>
           <c:idx val="8"/>
           <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$29</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1024*8</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr/>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$29:$G$29</c:f>
+              <c:f>'02.28 kernel launch'!$B$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.877697841726619</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97864768683274</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.964679911699779</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1024*16</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr/>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$30:$G$30</c:f>
+              <c:f>'02.28 kernel launch'!$B$28:$G$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.884892086330935</c:v>
+                  <c:v>0.59136690647482</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.941874258600237</c:v>
+                  <c:v>0.830367734282325</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.999779249448124</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.999574468085106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$31</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1024*32</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr/>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20:$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128 (8.4Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256 (4.5Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512 (2.35Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024 (1.2Mpps)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1514 (0.8 Mpps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$31:$G$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.902877697841727</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4962,7 +4809,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <c:date1904 val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5022,11 +4869,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$B$20</c:f>
+              <c:f>'02.28 kernel launch'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>64 (13.8~14.0Mpps)</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5035,83 +4882,83 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:f>'02.28 kernel launch'!$A$20:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>512</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1024</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1024*2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024*4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1024*8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024*16</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024*32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$B$21:$B$31</c:f>
+              <c:f>'02.28 kernel launch'!$B$20:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.0915827338129496</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>0.169352517985612</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>0.297841726618705</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>0.461151079136691</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>0.59136690647482</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>0.762589928057554</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>0.856115107913669</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.870503597122302</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.877697841726619</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.884892086330935</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.902877697841727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5122,11 +4969,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$C$20</c:f>
+              <c:f>'02.28 kernel launch'!$C$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>128 (8.4Mpps)</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5135,83 +4982,83 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:f>'02.28 kernel launch'!$A$20:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>512</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1024</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1024*2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024*4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1024*8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024*16</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024*32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$C$21:$C$31</c:f>
+              <c:f>'02.28 kernel launch'!$C$20:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.149466192170819</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>0.270462633451957</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>0.429418742586002</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>0.601423487544484</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>0.830367734282325</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>0.972716488730724</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.981020166073547</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.97864768683274</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.941874258600237</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5222,11 +5069,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$D$20</c:f>
+              <c:f>'02.28 kernel launch'!$D$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>256 (4.5Mpps)</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5235,83 +5082,83 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:f>'02.28 kernel launch'!$A$20:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>512</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1024</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1024*2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024*4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1024*8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024*16</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024*32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$D$21:$D$31</c:f>
+              <c:f>'02.28 kernel launch'!$D$20:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.269094922737307</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>0.463576158940397</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>0.649006622516556</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>0.960264900662252</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>0.999779249448124</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>0.999779249448124</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.964679911699779</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5322,11 +5169,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$E$20</c:f>
+              <c:f>'02.28 kernel launch'!$E$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>512 (2.35Mpps)</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5335,83 +5182,83 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:f>'02.28 kernel launch'!$A$20:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>512</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1024</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1024*2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024*4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1024*8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024*16</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024*32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$E$21:$E$31</c:f>
+              <c:f>'02.28 kernel launch'!$E$20:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.474893617021277</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>0.659574468085106</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>0.991489361702128</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>0.999574468085106</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>0.999574468085106</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5422,11 +5269,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$F$20</c:f>
+              <c:f>'02.28 kernel launch'!$F$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1024 (1.2Mpps)</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5435,65 +5282,65 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:f>'02.28 kernel launch'!$A$20:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>512</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1024</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1024*2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024*4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1024*8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024*16</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024*32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$F$21:$F$31</c:f>
+              <c:f>'02.28 kernel launch'!$F$20:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.672096908939014</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -5502,16 +5349,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5522,11 +5369,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$G$20</c:f>
+              <c:f>'02.28 kernel launch'!$G$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1514 (0.8 Mpps)</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5535,80 +5382,80 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'02.28 kernel launch'!$A$21:$A$31</c:f>
+              <c:f>'02.28 kernel launch'!$A$20:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>128</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>512</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1024</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1024*2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024*4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1024*8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024*16</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024*32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'02.28 kernel launch'!$G$21:$G$31</c:f>
+              <c:f>'02.28 kernel launch'!$G$20:$G$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.862576687116564</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>0.999754601226994</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>0.999754601226994</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>0.999877300613497</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -5694,7 +5541,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5759,7 +5606,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5884,7 +5731,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5906,7 +5753,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="12592051" cy="6086475"/>
+        <a:ext cx="12592051" cy="6086474"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5936,7 +5783,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="6791325"/>
-        <a:ext cx="12592051" cy="6086475"/>
+        <a:ext cx="12592051" cy="6086474"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6218,7 +6065,7 @@
   <x:sheetData>
     <x:row r="1" spans="2:7">
       <x:c r="B1" s="7" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C1" s="8"/>
       <x:c r="D1" s="8"/>
@@ -6243,16 +6090,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E3" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F3" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G3" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
@@ -6395,7 +6242,7 @@
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="A10" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B10" s="1">
         <x:v>13390000</x:v>
@@ -6416,7 +6263,7 @@
     </x:row>
     <x:row r="11" spans="1:7">
       <x:c r="A11" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B11" s="1">
         <x:v>12500000</x:v>
@@ -6435,7 +6282,7 @@
     </x:row>
     <x:row r="12" spans="1:7">
       <x:c r="A12" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B12" s="1">
         <x:v>12550000</x:v>
@@ -6452,7 +6299,7 @@
     </x:row>
     <x:row r="13" spans="1:7">
       <x:c r="A13" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B13" s="1">
         <x:v>12480000</x:v>
@@ -6467,7 +6314,7 @@
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B14" s="1">
         <x:v>12770000</x:v>
@@ -6480,7 +6327,7 @@
     </x:row>
     <x:row r="18" spans="2:7">
       <x:c r="B18" s="7" t="s">
-        <x:v>28</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C18" s="8"/>
       <x:c r="D18" s="8"/>
@@ -6505,16 +6352,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D20" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E20" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F20" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G20" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:7">
@@ -6693,7 +6540,7 @@
     </x:row>
     <x:row r="27" spans="1:7">
       <x:c r="A27" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B27" s="1">
         <x:f t="shared" si="3"/>
@@ -6719,7 +6566,7 @@
     </x:row>
     <x:row r="28" spans="1:7">
       <x:c r="A28" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B28" s="1">
         <x:f t="shared" si="3"/>
@@ -6742,7 +6589,7 @@
     </x:row>
     <x:row r="29" spans="1:7">
       <x:c r="A29" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B29" s="1">
         <x:f t="shared" si="3"/>
@@ -6765,7 +6612,7 @@
     </x:row>
     <x:row r="30" spans="1:7">
       <x:c r="A30" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B30" s="1">
         <x:f t="shared" si="3"/>
@@ -6788,7 +6635,7 @@
     </x:row>
     <x:row r="31" spans="1:7">
       <x:c r="A31" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B31" s="1">
         <x:f t="shared" si="3"/>
@@ -6820,7 +6667,7 @@
     </x:row>
     <x:row r="34" spans="2:7">
       <x:c r="B34" s="7" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C34" s="8"/>
       <x:c r="D34" s="8"/>
@@ -6845,16 +6692,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D36" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E36" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F36" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G36" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:7">
@@ -6997,7 +6844,7 @@
     </x:row>
     <x:row r="43" spans="1:7">
       <x:c r="A43" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B43" s="1">
         <x:v>6420</x:v>
@@ -7018,7 +6865,7 @@
     </x:row>
     <x:row r="44" spans="1:7">
       <x:c r="A44" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B44" s="1">
         <x:v>3050</x:v>
@@ -7037,7 +6884,7 @@
     </x:row>
     <x:row r="45" spans="1:7">
       <x:c r="A45" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B45" s="1">
         <x:v>1532</x:v>
@@ -7054,7 +6901,7 @@
     </x:row>
     <x:row r="46" spans="1:7">
       <x:c r="A46" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B46" s="1">
         <x:v>760</x:v>
@@ -7069,7 +6916,7 @@
     </x:row>
     <x:row r="47" spans="1:7">
       <x:c r="A47" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B47" s="1">
         <x:v>387</x:v>
@@ -7141,8 +6988,8 @@
   <x:sheetPr codeName="Sheet2"/>
   <x:dimension ref="A1:M58"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="G1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="A1" activeCellId="0" sqref="A1:G19"/>
+    <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="G23" activeCellId="0" sqref="A22:G23"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.550000000000001"/>
@@ -7153,10 +7000,10 @@
   <x:sheetData>
     <x:row r="1" spans="2:7" customHeight="1">
       <x:c r="B1" s="10" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C1" s="10" t="s">
-        <x:v>27</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D1" s="10" t="s">
         <x:v>18</x:v>
@@ -7165,10 +7012,10 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="F1" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="G1" s="10" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="G1" s="10" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="2:13" customHeight="1">
@@ -7325,7 +7172,7 @@
     </x:row>
     <x:row r="9" spans="1:7" customHeight="1">
       <x:c r="A9" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B9" s="4">
         <x:v>2722</x:v>
@@ -7348,7 +7195,7 @@
     </x:row>
     <x:row r="10" spans="1:7" customHeight="1">
       <x:c r="A10" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B10" s="4">
         <x:v>2843</x:v>
@@ -7371,7 +7218,7 @@
     </x:row>
     <x:row r="11" spans="1:7" customHeight="1">
       <x:c r="A11" s="1" t="s">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B11" s="4">
         <x:v>3133</x:v>
@@ -7394,7 +7241,7 @@
     </x:row>
     <x:row r="12" spans="1:7" customHeight="1">
       <x:c r="A12" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B12" s="4">
         <x:v>3857</x:v>
@@ -7417,7 +7264,7 @@
     </x:row>
     <x:row r="13" spans="1:7" customHeight="1">
       <x:c r="A13" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B13" s="4">
         <x:v>5125</x:v>
@@ -7440,7 +7287,7 @@
     </x:row>
     <x:row r="14" spans="1:7" customHeight="1">
       <x:c r="A14" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B14" s="4">
         <x:v>7528</x:v>
@@ -7463,7 +7310,7 @@
     </x:row>
     <x:row r="15" spans="1:7" customHeight="1">
       <x:c r="A15" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B15" s="4">
         <x:v>11994</x:v>
@@ -7486,7 +7333,7 @@
     </x:row>
     <x:row r="16" spans="1:7" customHeight="1">
       <x:c r="A16" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B16" s="4">
         <x:v>19883</x:v>
@@ -7509,7 +7356,7 @@
     </x:row>
     <x:row r="17" spans="1:7" customHeight="1">
       <x:c r="A17" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B17" s="4">
         <x:v>37751</x:v>
@@ -7532,7 +7379,7 @@
     </x:row>
     <x:row r="18" spans="1:7" customHeight="1">
       <x:c r="A18" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B18" s="4">
         <x:v>85677</x:v>
@@ -7555,7 +7402,7 @@
     </x:row>
     <x:row r="19" spans="1:7" customHeight="1">
       <x:c r="A19" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B19" s="4">
         <x:v>206878</x:v>
@@ -7669,59 +7516,59 @@
     </x:row>
     <x:row r="48" spans="1:4">
       <x:c r="A48" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B48" s="3"/>
       <x:c r="D48" s="3"/>
     </x:row>
     <x:row r="49" spans="1:1">
       <x:c r="A49" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:1">
       <x:c r="A50" s="1" t="s">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:1">
       <x:c r="A51" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:1">
       <x:c r="A52" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:1">
       <x:c r="A53" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:1">
       <x:c r="A54" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:1">
       <x:c r="A55" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:1">
       <x:c r="A56" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:1">
       <x:c r="A57" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:1">
       <x:c r="A58" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -7758,7 +7605,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="11" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B1" s="9"/>
       <x:c r="C1" s="9"/>
@@ -7774,10 +7621,10 @@
     </x:row>
     <x:row r="3" spans="2:5">
       <x:c r="B3" s="10" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C3" s="10" t="s">
-        <x:v>27</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D3" s="10" t="s">
         <x:v>18</x:v>
@@ -7896,7 +7743,7 @@
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B11" s="4">
         <x:v>7445</x:v>
@@ -7913,7 +7760,7 @@
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B12" s="4">
         <x:v>2307</x:v>
@@ -7930,7 +7777,7 @@
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="1" t="s">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B13" s="4">
         <x:v>3334</x:v>
@@ -7947,7 +7794,7 @@
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="A14" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B14" s="4">
         <x:v>5643</x:v>
@@ -7964,7 +7811,7 @@
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="A15" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B15" s="4">
         <x:v>8649</x:v>
@@ -7981,7 +7828,7 @@
     </x:row>
     <x:row r="16" spans="1:5">
       <x:c r="A16" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B16" s="4">
         <x:v>7925</x:v>
@@ -7998,7 +7845,7 @@
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="A17" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B17" s="4">
         <x:v>19881</x:v>
@@ -8015,7 +7862,7 @@
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="A18" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B18" s="4">
         <x:v>26627</x:v>
@@ -8032,7 +7879,7 @@
     </x:row>
     <x:row r="19" spans="1:5">
       <x:c r="A19" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B19" s="4">
         <x:v>40525</x:v>
@@ -8049,7 +7896,7 @@
     </x:row>
     <x:row r="20" spans="1:5">
       <x:c r="A20" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B20" s="4">
         <x:v>74741</x:v>
@@ -8066,7 +7913,7 @@
     </x:row>
     <x:row r="21" spans="1:5">
       <x:c r="A21" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B21" s="4">
         <x:v>150490</x:v>
@@ -8083,7 +7930,7 @@
     </x:row>
     <x:row r="25" spans="1:5" ht="24.949999999999999" customHeight="1">
       <x:c r="A25" s="11" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B25" s="9"/>
       <x:c r="C25" s="9"/>
@@ -8099,10 +7946,10 @@
     </x:row>
     <x:row r="27" spans="2:3">
       <x:c r="B27" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C27" s="10" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="C27" s="10" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="2:3">
@@ -8177,7 +8024,7 @@
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B35">
         <x:v>1704662</x:v>
@@ -8188,7 +8035,7 @@
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B36">
         <x:v>888145</x:v>
@@ -8199,7 +8046,7 @@
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="A37" s="1" t="s">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B37">
         <x:v>501401</x:v>
@@ -8210,7 +8057,7 @@
     </x:row>
     <x:row r="38" spans="1:3">
       <x:c r="A38" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B38">
         <x:v>332799</x:v>
@@ -8221,7 +8068,7 @@
     </x:row>
     <x:row r="39" spans="1:3">
       <x:c r="A39" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B39">
         <x:v>234809</x:v>
@@ -8232,7 +8079,7 @@
     </x:row>
     <x:row r="40" spans="1:3">
       <x:c r="A40" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B40">
         <x:v>185326</x:v>
@@ -8243,7 +8090,7 @@
     </x:row>
     <x:row r="41" spans="1:3">
       <x:c r="A41" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B41">
         <x:v>161905</x:v>
@@ -8254,7 +8101,7 @@
     </x:row>
     <x:row r="42" spans="1:3">
       <x:c r="A42" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B42">
         <x:v>150163</x:v>
@@ -8265,7 +8112,7 @@
     </x:row>
     <x:row r="43" spans="1:3">
       <x:c r="A43" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B43">
         <x:v>145611</x:v>
@@ -8276,7 +8123,7 @@
     </x:row>
     <x:row r="44" spans="1:3">
       <x:c r="A44" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B44">
         <x:v>148653</x:v>
@@ -8287,7 +8134,7 @@
     </x:row>
     <x:row r="45" spans="1:3">
       <x:c r="A45" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B45">
         <x:v>167357</x:v>
@@ -8298,7 +8145,7 @@
     </x:row>
     <x:row r="48" spans="1:7" ht="24.949999999999999" customHeight="1">
       <x:c r="A48" s="11" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B48" s="7"/>
       <x:c r="C48" s="7"/>
@@ -8318,10 +8165,10 @@
     </x:row>
     <x:row r="50" spans="2:5">
       <x:c r="B50" s="10" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C50" s="10" t="s">
-        <x:v>27</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D50" s="10" t="s">
         <x:v>18</x:v>
@@ -8440,7 +8287,7 @@
     </x:row>
     <x:row r="58" spans="1:5">
       <x:c r="A58" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B58" s="4">
         <x:v>2330</x:v>
@@ -8457,7 +8304,7 @@
     </x:row>
     <x:row r="59" spans="1:5">
       <x:c r="A59" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B59" s="4">
         <x:v>3582</x:v>
@@ -8474,7 +8321,7 @@
     </x:row>
     <x:row r="60" spans="1:5">
       <x:c r="A60" s="1" t="s">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B60" s="4">
         <x:v>3213</x:v>
@@ -8491,7 +8338,7 @@
     </x:row>
     <x:row r="61" spans="1:5">
       <x:c r="A61" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B61" s="4">
         <x:v>3588</x:v>
@@ -8508,7 +8355,7 @@
     </x:row>
     <x:row r="62" spans="1:5">
       <x:c r="A62" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B62" s="5">
         <x:v>12283</x:v>
@@ -8525,7 +8372,7 @@
     </x:row>
     <x:row r="63" spans="1:5">
       <x:c r="A63" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B63" s="4">
         <x:v>7954</x:v>
@@ -8542,7 +8389,7 @@
     </x:row>
     <x:row r="64" spans="1:5">
       <x:c r="A64" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B64" s="4">
         <x:v>11599</x:v>
@@ -8559,7 +8406,7 @@
     </x:row>
     <x:row r="65" spans="1:5">
       <x:c r="A65" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B65" s="4">
         <x:v>20553</x:v>
@@ -8576,7 +8423,7 @@
     </x:row>
     <x:row r="66" spans="1:5">
       <x:c r="A66" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B66" s="4">
         <x:v>38486</x:v>
@@ -8593,7 +8440,7 @@
     </x:row>
     <x:row r="67" spans="1:5">
       <x:c r="A67" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B67" s="4">
         <x:v>75167</x:v>
@@ -8610,7 +8457,7 @@
     </x:row>
     <x:row r="68" spans="1:5">
       <x:c r="A68" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B68" s="4">
         <x:v>161317</x:v>
@@ -8627,7 +8474,7 @@
     </x:row>
     <x:row r="73" spans="1:5" ht="24.949999999999999" customHeight="1">
       <x:c r="A73" s="11" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B73" s="7"/>
       <x:c r="C73" s="7"/>
@@ -8643,10 +8490,10 @@
     </x:row>
     <x:row r="75" spans="2:3">
       <x:c r="B75" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C75" s="10" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="C75" s="10" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="2:3">
@@ -8721,7 +8568,7 @@
     </x:row>
     <x:row r="83" spans="1:3">
       <x:c r="A83" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B83">
         <x:v>1708597</x:v>
@@ -8732,7 +8579,7 @@
     </x:row>
     <x:row r="84" spans="1:3">
       <x:c r="A84" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B84">
         <x:v>889942</x:v>
@@ -8743,7 +8590,7 @@
     </x:row>
     <x:row r="85" spans="1:3">
       <x:c r="A85" s="1" t="s">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B85">
         <x:v>506309</x:v>
@@ -8754,7 +8601,7 @@
     </x:row>
     <x:row r="86" spans="1:3">
       <x:c r="A86" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B86">
         <x:v>344510</x:v>
@@ -8765,7 +8612,7 @@
     </x:row>
     <x:row r="87" spans="1:3">
       <x:c r="A87" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B87">
         <x:v>242647</x:v>
@@ -8776,7 +8623,7 @@
     </x:row>
     <x:row r="88" spans="1:3">
       <x:c r="A88" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B88">
         <x:v>185274</x:v>
@@ -8787,7 +8634,7 @@
     </x:row>
     <x:row r="89" spans="1:3">
       <x:c r="A89" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B89">
         <x:v>158391</x:v>
@@ -8798,7 +8645,7 @@
     </x:row>
     <x:row r="90" spans="1:3">
       <x:c r="A90" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B90">
         <x:v>149039</x:v>
@@ -8809,7 +8656,7 @@
     </x:row>
     <x:row r="91" spans="1:3">
       <x:c r="A91" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B91">
         <x:v>153874</x:v>
@@ -8820,7 +8667,7 @@
     </x:row>
     <x:row r="92" spans="1:3">
       <x:c r="A92" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B92">
         <x:v>154735</x:v>
@@ -8831,7 +8678,7 @@
     </x:row>
     <x:row r="93" spans="1:3">
       <x:c r="A93" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B93">
         <x:v>169481</x:v>
@@ -8884,10 +8731,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet5"/>
-  <x:dimension ref="A1:G47"/>
+  <x:dimension ref="A1:H58"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="H16" activeCellId="0" sqref="H16:H16"/>
+    <x:sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="H36" activeCellId="0" sqref="H36:H36"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.550000000000001"/>
@@ -8898,7 +8745,7 @@
   <x:sheetData>
     <x:row r="1" spans="2:7">
       <x:c r="B1" s="7" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C1" s="8"/>
       <x:c r="D1" s="8"/>
@@ -8923,16 +8770,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E3" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F3" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G3" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
@@ -9075,7 +8922,7 @@
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="A10" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B10" s="1">
         <x:v>11900000</x:v>
@@ -9096,7 +8943,7 @@
     </x:row>
     <x:row r="11" spans="1:7">
       <x:c r="A11" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B11" s="1">
         <x:v>12100000</x:v>
@@ -9115,7 +8962,7 @@
     </x:row>
     <x:row r="12" spans="1:7">
       <x:c r="A12" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B12" s="1">
         <x:v>12200000</x:v>
@@ -9132,7 +8979,7 @@
     </x:row>
     <x:row r="13" spans="1:7">
       <x:c r="A13" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B13" s="1">
         <x:v>12300000</x:v>
@@ -9147,653 +8994,801 @@
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B14" s="1">
         <x:v>12550000</x:v>
       </x:c>
-      <x:c r="C14" s="1"/>
+      <x:c r="C14" s="1">
+        <x:v>7500000</x:v>
+      </x:c>
       <x:c r="D14" s="1"/>
       <x:c r="E14" s="1"/>
       <x:c r="F14" s="1"/>
       <x:c r="G14" s="1"/>
     </x:row>
-    <x:row r="18" spans="2:7">
-      <x:c r="B18" s="7" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C18" s="8"/>
-      <x:c r="D18" s="8"/>
-      <x:c r="E18" s="8"/>
-      <x:c r="F18" s="8"/>
-      <x:c r="G18" s="8"/>
-    </x:row>
-    <x:row r="19" spans="2:7">
-      <x:c r="B19" s="8"/>
-      <x:c r="C19" s="8"/>
-      <x:c r="D19" s="8"/>
-      <x:c r="E19" s="8"/>
-      <x:c r="F19" s="8"/>
-      <x:c r="G19" s="8"/>
-    </x:row>
-    <x:row r="20" spans="1:7">
-      <x:c r="A20" s="1"/>
-      <x:c r="B20" s="1" t="s">
+    <x:row r="15" spans="1:3">
+      <x:c r="A15" s="1" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B15">
+        <x:v>12500000</x:v>
+      </x:c>
+      <x:c r="C15">
+        <x:v>7100000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:3">
+      <x:c r="A16" s="1" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B16">
+        <x:v>12000000</x:v>
+      </x:c>
+      <x:c r="C16">
+        <x:v>6700000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:3">
+      <x:c r="A17" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B17">
+        <x:v>11200000</x:v>
+      </x:c>
+      <x:c r="C17">
+        <x:v>7940000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:2">
+      <x:c r="A18" s="1" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B18">
+        <x:v>11500000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="2:7">
+      <x:c r="B21" s="7" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C21" s="8"/>
+      <x:c r="D21" s="8"/>
+      <x:c r="E21" s="8"/>
+      <x:c r="F21" s="8"/>
+      <x:c r="G21" s="8"/>
+    </x:row>
+    <x:row r="22" spans="2:7">
+      <x:c r="B22" s="8"/>
+      <x:c r="C22" s="8"/>
+      <x:c r="D22" s="8"/>
+      <x:c r="E22" s="8"/>
+      <x:c r="F22" s="8"/>
+      <x:c r="G22" s="8"/>
+    </x:row>
+    <x:row r="23" spans="1:7">
+      <x:c r="A23" s="1"/>
+      <x:c r="B23" s="1" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C20" s="1" t="s">
+      <x:c r="C23" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D20" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="E20" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F20" s="1" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G20" s="1" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:7">
-      <x:c r="A21" s="1">
+      <x:c r="D23" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E23" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F23" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G23" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:7">
+      <x:c r="A24" s="1">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="B21" s="1">
+      <x:c r="B24" s="12">
         <x:f>B4/13900000</x:f>
         <x:v>0.091582733812949638</x:v>
       </x:c>
-      <x:c r="C21">
+      <x:c r="C24" s="13">
         <x:f>C4/MAX($C$4:$C$13)</x:f>
         <x:v>0.1494661921708185</x:v>
       </x:c>
-      <x:c r="D21">
+      <x:c r="D24" s="13">
         <x:f>D4/MAX($D$4:$D$13)</x:f>
         <x:v>0.26909492273730684</x:v>
       </x:c>
-      <x:c r="E21">
+      <x:c r="E24" s="13">
         <x:f>E4/MAX($E$4:$E$13)</x:f>
         <x:v>0.47489361702127658</x:v>
       </x:c>
-      <x:c r="F21">
+      <x:c r="F24" s="13">
         <x:f>F4/MAX($F$4:$F$13)</x:f>
         <x:v>0.67209690893901419</x:v>
       </x:c>
-      <x:c r="G21">
+      <x:c r="G24" s="13">
         <x:f>G4/MAX($G$4:$G$13)</x:f>
         <x:v>0.86257668711656443</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:7">
-      <x:c r="A22" s="1">
+    <x:row r="25" spans="1:7">
+      <x:c r="A25" s="1">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="B22" s="1">
-        <x:f t="shared" ref="B22:B31" si="0">B5/13900000</x:f>
+      <x:c r="B25" s="12">
+        <x:f t="shared" ref="B25:B38" si="0">B5/13900000</x:f>
         <x:v>0.16935251798561152</x:v>
       </x:c>
-      <x:c r="C22">
-        <x:f t="shared" ref="C22:C31" si="1">C5/MAX($C$4:$C$13)</x:f>
+      <x:c r="C25" s="13">
+        <x:f t="shared" ref="C25:C38" si="1">C5/MAX($C$4:$C$13)</x:f>
         <x:v>0.27046263345195731</x:v>
       </x:c>
-      <x:c r="D22">
-        <x:f t="shared" ref="D22:D31" si="2">D5/MAX($D$4:$D$13)</x:f>
+      <x:c r="D25" s="13">
+        <x:f t="shared" ref="D25:D34" si="2">D5/MAX($D$4:$D$13)</x:f>
         <x:v>0.46357615894039733</x:v>
       </x:c>
-      <x:c r="E22">
-        <x:f t="shared" ref="E22:E31" si="3">E5/MAX($E$4:$E$13)</x:f>
+      <x:c r="E25" s="13">
+        <x:f t="shared" ref="E25:E34" si="3">E5/MAX($E$4:$E$13)</x:f>
         <x:v>0.65957446808510634</x:v>
       </x:c>
-      <x:c r="F22">
-        <x:f t="shared" ref="F22:F31" si="4">F5/MAX($F$4:$F$13)</x:f>
+      <x:c r="F25" s="13">
+        <x:f t="shared" ref="F25:F34" si="4">F5/MAX($F$4:$F$13)</x:f>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="G22">
-        <x:f t="shared" ref="G22:G31" si="5">G5/MAX($G$4:$G$13)</x:f>
+      <x:c r="G25" s="13">
+        <x:f t="shared" ref="G25:G34" si="5">G5/MAX($G$4:$G$13)</x:f>
         <x:v>0.99975460122699389</x:v>
       </x:c>
     </x:row>
-    <x:row r="23" spans="1:7">
-      <x:c r="A23" s="1">
+    <x:row r="26" spans="1:7">
+      <x:c r="A26" s="1">
         <x:v>128</x:v>
       </x:c>
-      <x:c r="B23" s="1">
+      <x:c r="B26" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.29784172661870506</x:v>
       </x:c>
-      <x:c r="C23">
+      <x:c r="C26" s="13">
         <x:f t="shared" si="1"/>
         <x:v>0.42941874258600238</x:v>
       </x:c>
-      <x:c r="D23">
+      <x:c r="D26" s="13">
         <x:f t="shared" si="2"/>
         <x:v>0.64900662251655628</x:v>
       </x:c>
-      <x:c r="E23">
+      <x:c r="E26" s="13">
         <x:f t="shared" si="3"/>
         <x:v>0.99148936170212765</x:v>
       </x:c>
-      <x:c r="F23">
+      <x:c r="F26" s="13">
         <x:f t="shared" si="4"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="G23">
+      <x:c r="G26" s="13">
         <x:f t="shared" si="5"/>
         <x:v>0.99975460122699389</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:7">
-      <x:c r="A24" s="1">
+    <x:row r="27" spans="1:7">
+      <x:c r="A27" s="1">
         <x:v>256</x:v>
       </x:c>
-      <x:c r="B24" s="1">
+      <x:c r="B27" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.46115107913669062</x:v>
       </x:c>
-      <x:c r="C24">
+      <x:c r="C27" s="13">
         <x:f t="shared" si="1"/>
         <x:v>0.60142348754448394</x:v>
       </x:c>
-      <x:c r="D24">
+      <x:c r="D27" s="13">
         <x:f t="shared" si="2"/>
         <x:v>0.96026490066225167</x:v>
       </x:c>
-      <x:c r="E24">
+      <x:c r="E27" s="13">
         <x:f t="shared" si="3"/>
         <x:v>0.99957446808510642</x:v>
       </x:c>
-      <x:c r="F24">
+      <x:c r="F27" s="13">
         <x:f t="shared" si="4"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="G24">
+      <x:c r="G27" s="13">
         <x:f t="shared" si="5"/>
         <x:v>0.99987730061349689</x:v>
       </x:c>
     </x:row>
-    <x:row r="25" spans="1:7">
-      <x:c r="A25" s="1">
+    <x:row r="28" spans="1:7">
+      <x:c r="A28" s="1">
         <x:v>512</x:v>
       </x:c>
-      <x:c r="B25" s="1">
+      <x:c r="B28" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.59136690647482015</x:v>
       </x:c>
-      <x:c r="C25">
+      <x:c r="C28" s="13">
         <x:f t="shared" si="1"/>
         <x:v>0.83036773428232502</x:v>
       </x:c>
-      <x:c r="D25">
+      <x:c r="D28" s="13">
         <x:f t="shared" si="2"/>
         <x:v>0.99977924944812357</x:v>
       </x:c>
-      <x:c r="E25">
+      <x:c r="E28" s="13">
         <x:f t="shared" si="3"/>
         <x:v>0.99957446808510642</x:v>
       </x:c>
-      <x:c r="F25">
+      <x:c r="F28" s="13">
         <x:f t="shared" si="4"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="G25">
+      <x:c r="G28" s="13">
         <x:f t="shared" si="5"/>
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="26" spans="1:7">
-      <x:c r="A26" s="1">
+    <x:row r="29" spans="1:7">
+      <x:c r="A29" s="1">
         <x:v>1024</x:v>
       </x:c>
-      <x:c r="B26" s="1">
+      <x:c r="B29" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.76258992805755399</x:v>
       </x:c>
-      <x:c r="C26">
+      <x:c r="C29" s="13">
         <x:f t="shared" si="1"/>
         <x:v>0.97271648873072358</x:v>
       </x:c>
-      <x:c r="D26">
+      <x:c r="D29" s="13">
         <x:f t="shared" si="2"/>
         <x:v>0.99977924944812357</x:v>
       </x:c>
-      <x:c r="E26">
+      <x:c r="E29" s="13">
         <x:f t="shared" si="3"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="F26">
+      <x:c r="F29" s="13">
         <x:f t="shared" si="4"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="G26">
+      <x:c r="G29" s="13">
         <x:f t="shared" si="5"/>
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="27" spans="1:7">
-      <x:c r="A27" s="1" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B27" s="1">
+    <x:row r="30" spans="1:7">
+      <x:c r="A30" s="1" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B30" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.85611510791366907</x:v>
       </x:c>
-      <x:c r="C27">
+      <x:c r="C30" s="13">
         <x:f t="shared" si="1"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="D27">
+      <x:c r="D30" s="13">
         <x:f t="shared" si="2"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E27">
+      <x:c r="E30" s="13">
         <x:f t="shared" si="3"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="F27">
+      <x:c r="F30" s="13">
         <x:f t="shared" si="4"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="G27">
+      <x:c r="G30" s="13">
         <x:f t="shared" si="5"/>
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="28" spans="1:7">
-      <x:c r="A28" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B28" s="1">
+    <x:row r="31" spans="1:7">
+      <x:c r="A31" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B31" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.87050359712230219</x:v>
       </x:c>
-      <x:c r="C28">
+      <x:c r="C31" s="13">
         <x:f t="shared" si="1"/>
         <x:v>0.98102016607354681</x:v>
       </x:c>
-      <x:c r="D28">
+      <x:c r="D31" s="13">
         <x:f t="shared" si="2"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E28">
+      <x:c r="E31" s="13">
         <x:f t="shared" si="3"/>
         <x:v>1</x:v>
       </x:c>
-      <x:c r="F28">
+      <x:c r="F31" s="13">
         <x:f t="shared" si="4"/>
         <x:v>0</x:v>
       </x:c>
-      <x:c r="G28">
+      <x:c r="G31" s="13">
         <x:f t="shared" si="5"/>
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="29" spans="1:7">
-      <x:c r="A29" s="1" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B29" s="1">
+    <x:row r="32" spans="1:7">
+      <x:c r="A32" s="1" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B32" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.87769784172661869</x:v>
       </x:c>
-      <x:c r="C29">
+      <x:c r="C32" s="13">
         <x:f t="shared" si="1"/>
         <x:v>0.97864768683274017</x:v>
       </x:c>
-      <x:c r="D29">
+      <x:c r="D32" s="13">
         <x:f t="shared" si="2"/>
         <x:v>0.96467991169977929</x:v>
       </x:c>
-      <x:c r="E29">
+      <x:c r="E32" s="13">
         <x:f t="shared" si="3"/>
         <x:v>0</x:v>
       </x:c>
-      <x:c r="F29">
+      <x:c r="F32" s="13">
         <x:f t="shared" si="4"/>
         <x:v>0</x:v>
       </x:c>
-      <x:c r="G29">
+      <x:c r="G32" s="13">
         <x:f t="shared" si="5"/>
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="30" spans="1:7">
-      <x:c r="A30" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B30" s="1">
+    <x:row r="33" spans="1:7">
+      <x:c r="A33" s="1" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B33" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.8848920863309353</x:v>
       </x:c>
-      <x:c r="C30">
+      <x:c r="C33" s="13">
         <x:f t="shared" si="1"/>
         <x:v>0.94187425860023721</x:v>
       </x:c>
-      <x:c r="D30">
+      <x:c r="D33" s="13">
         <x:f t="shared" si="2"/>
         <x:v>0</x:v>
       </x:c>
-      <x:c r="E30">
+      <x:c r="E33" s="13">
         <x:f t="shared" si="3"/>
         <x:v>0</x:v>
       </x:c>
-      <x:c r="F30">
+      <x:c r="F33" s="13">
         <x:f t="shared" si="4"/>
         <x:v>0</x:v>
       </x:c>
-      <x:c r="G30">
+      <x:c r="G33" s="13">
         <x:f t="shared" si="5"/>
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="31" spans="1:7">
-      <x:c r="A31" s="1" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="B31" s="1">
+    <x:row r="34" spans="1:7">
+      <x:c r="A34" s="1" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B34" s="12">
         <x:f t="shared" si="0"/>
         <x:v>0.90287769784172667</x:v>
       </x:c>
-      <x:c r="C31">
+      <x:c r="C34" s="13">
+        <x:f t="shared" si="1"/>
+        <x:v>0.88967971530249113</x:v>
+      </x:c>
+      <x:c r="D34" s="13">
+        <x:f t="shared" si="2"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E34" s="13">
+        <x:f t="shared" si="3"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F34" s="13">
+        <x:f t="shared" si="4"/>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G34" s="13">
+        <x:f t="shared" si="5"/>
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:7">
+      <x:c r="A35" s="1" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B35" s="12">
+        <x:f t="shared" si="0"/>
+        <x:v>0.89928057553956831</x:v>
+      </x:c>
+      <x:c r="C35" s="13">
+        <x:f t="shared" si="1"/>
+        <x:v>0.8422301304863582</x:v>
+      </x:c>
+      <x:c r="D35" s="13"/>
+      <x:c r="E35" s="13"/>
+      <x:c r="F35" s="13"/>
+      <x:c r="G35" s="13"/>
+    </x:row>
+    <x:row r="36" spans="1:8">
+      <x:c r="A36" s="1" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B36" s="12">
+        <x:f t="shared" si="0"/>
+        <x:v>0.86330935251798557</x:v>
+      </x:c>
+      <x:c r="C36" s="13">
+        <x:f t="shared" si="1"/>
+        <x:v>0.79478054567022538</x:v>
+      </x:c>
+      <x:c r="D36" s="13"/>
+      <x:c r="E36" s="13"/>
+      <x:c r="F36" s="13"/>
+      <x:c r="G36" s="13"/>
+      <x:c r="H36" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:7">
+      <x:c r="A37" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B37" s="12">
+        <x:f t="shared" si="0"/>
+        <x:v>0.80575539568345322</x:v>
+      </x:c>
+      <x:c r="C37" s="13">
+        <x:f t="shared" si="1"/>
+        <x:v>0.94187425860023721</x:v>
+      </x:c>
+      <x:c r="D37" s="13"/>
+      <x:c r="E37" s="13"/>
+      <x:c r="F37" s="13"/>
+      <x:c r="G37" s="13"/>
+    </x:row>
+    <x:row r="38" spans="1:7">
+      <x:c r="A38" s="1" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B38" s="12">
+        <x:f t="shared" si="0"/>
+        <x:v>0.82733812949640284</x:v>
+      </x:c>
+      <x:c r="C38" s="13">
         <x:f t="shared" si="1"/>
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D31">
-        <x:f t="shared" si="2"/>
+      <x:c r="D38" s="13"/>
+      <x:c r="E38" s="13"/>
+      <x:c r="F38" s="13"/>
+      <x:c r="G38" s="13"/>
+    </x:row>
+    <x:row r="41" spans="2:7">
+      <x:c r="B41" s="7" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C41" s="8"/>
+      <x:c r="D41" s="8"/>
+      <x:c r="E41" s="8"/>
+      <x:c r="F41" s="8"/>
+      <x:c r="G41" s="8"/>
+    </x:row>
+    <x:row r="42" spans="2:7">
+      <x:c r="B42" s="8"/>
+      <x:c r="C42" s="8"/>
+      <x:c r="D42" s="8"/>
+      <x:c r="E42" s="8"/>
+      <x:c r="F42" s="8"/>
+      <x:c r="G42" s="8"/>
+    </x:row>
+    <x:row r="43" spans="1:7">
+      <x:c r="A43" s="1"/>
+      <x:c r="B43" s="1" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C43" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D43" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E43" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F43" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G43" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:7">
+      <x:c r="A44" s="1">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B44">
+        <x:v>39530</x:v>
+      </x:c>
+      <x:c r="C44" s="1">
+        <x:v>39470</x:v>
+      </x:c>
+      <x:c r="D44" s="1">
+        <x:v>38000</x:v>
+      </x:c>
+      <x:c r="E44" s="1">
+        <x:v>34000</x:v>
+      </x:c>
+      <x:c r="F44" s="1">
+        <x:v>25100</x:v>
+      </x:c>
+      <x:c r="G44" s="1">
+        <x:v>21970</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:7">
+      <x:c r="A45" s="1">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B45" s="1">
+        <x:v>36500</x:v>
+      </x:c>
+      <x:c r="C45" s="1">
+        <x:v>35600</x:v>
+      </x:c>
+      <x:c r="D45" s="1">
+        <x:v>32900</x:v>
+      </x:c>
+      <x:c r="E45" s="1">
+        <x:v>24270</x:v>
+      </x:c>
+      <x:c r="F45" s="1">
+        <x:v>18600</x:v>
+      </x:c>
+      <x:c r="G45" s="1">
+        <x:v>12700</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:7">
+      <x:c r="A46" s="1">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B46" s="1">
+        <x:v>31900</x:v>
+      </x:c>
+      <x:c r="C46" s="1">
+        <x:v>28400</x:v>
+      </x:c>
+      <x:c r="D46" s="1">
+        <x:v>22900</x:v>
+      </x:c>
+      <x:c r="E46" s="1">
+        <x:v>18200</x:v>
+      </x:c>
+      <x:c r="F46" s="1">
+        <x:v>9347</x:v>
+      </x:c>
+      <x:c r="G46" s="1">
+        <x:v>6363</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:7">
+      <x:c r="A47" s="1">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="B47" s="1">
+        <x:v>25133</x:v>
+      </x:c>
+      <x:c r="C47" s="1">
+        <x:v>19800</x:v>
+      </x:c>
+      <x:c r="D47" s="1">
+        <x:v>17000</x:v>
+      </x:c>
+      <x:c r="E47" s="1">
+        <x:v>9170</x:v>
+      </x:c>
+      <x:c r="F47" s="1">
+        <x:v>4676</x:v>
+      </x:c>
+      <x:c r="G47" s="1">
+        <x:v>3183</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:7">
+      <x:c r="A48" s="1">
+        <x:v>512</x:v>
+      </x:c>
+      <x:c r="B48" s="1">
+        <x:v>16000</x:v>
+      </x:c>
+      <x:c r="C48" s="1">
+        <x:v>13600</x:v>
+      </x:c>
+      <x:c r="D48" s="1">
+        <x:v>8846</x:v>
+      </x:c>
+      <x:c r="E48" s="1">
+        <x:v>4589</x:v>
+      </x:c>
+      <x:c r="F48" s="1">
+        <x:v>2339</x:v>
+      </x:c>
+      <x:c r="G48" s="1">
+        <x:v>1592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:7">
+      <x:c r="A49" s="1">
+        <x:v>1024</x:v>
+      </x:c>
+      <x:c r="B49" s="1">
+        <x:v>10425</x:v>
+      </x:c>
+      <x:c r="C49" s="1">
+        <x:v>8020</x:v>
+      </x:c>
+      <x:c r="D49" s="1">
+        <x:v>4423</x:v>
+      </x:c>
+      <x:c r="E49" s="1">
+        <x:v>2295</x:v>
+      </x:c>
+      <x:c r="F49" s="1">
+        <x:v>1169</x:v>
+      </x:c>
+      <x:c r="G49" s="1">
+        <x:v>796</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:7">
+      <x:c r="A50" s="1" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B50" s="1">
+        <x:v>5830</x:v>
+      </x:c>
+      <x:c r="C50" s="1">
+        <x:v>4113</x:v>
+      </x:c>
+      <x:c r="D50" s="1">
+        <x:v>2211</x:v>
+      </x:c>
+      <x:c r="E50" s="1">
+        <x:v>1147</x:v>
+      </x:c>
+      <x:c r="F50" s="1">
+        <x:v>585</x:v>
+      </x:c>
+      <x:c r="G50" s="1"/>
+    </x:row>
+    <x:row r="51" spans="1:7">
+      <x:c r="A51" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B51" s="1">
+        <x:v>2960</x:v>
+      </x:c>
+      <x:c r="C51" s="1">
+        <x:v>2020</x:v>
+      </x:c>
+      <x:c r="D51" s="1">
+        <x:v>1106</x:v>
+      </x:c>
+      <x:c r="E51" s="1">
+        <x:v>574</x:v>
+      </x:c>
+      <x:c r="F51" s="1"/>
+      <x:c r="G51" s="1"/>
+    </x:row>
+    <x:row r="52" spans="1:7">
+      <x:c r="A52" s="1" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B52" s="1">
+        <x:v>1490</x:v>
+      </x:c>
+      <x:c r="C52" s="1">
+        <x:v>1008</x:v>
+      </x:c>
+      <x:c r="D52" s="1">
+        <x:v>533</x:v>
+      </x:c>
+      <x:c r="E52" s="1"/>
+      <x:c r="F52" s="1"/>
+      <x:c r="G52" s="1"/>
+    </x:row>
+    <x:row r="53" spans="1:7">
+      <x:c r="A53" s="1" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B53" s="1">
+        <x:v>752</x:v>
+      </x:c>
+      <x:c r="C53" s="1">
+        <x:v>485</x:v>
+      </x:c>
+      <x:c r="D53" s="1"/>
+      <x:c r="E53" s="1"/>
+      <x:c r="F53" s="1"/>
+      <x:c r="G53" s="1"/>
+    </x:row>
+    <x:row r="54" spans="1:7">
+      <x:c r="A54" s="1" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B54" s="1">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="C54" s="1">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="D54" s="1"/>
+      <x:c r="E54" s="1"/>
+      <x:c r="F54" s="1"/>
+      <x:c r="G54" s="1"/>
+    </x:row>
+    <x:row r="55" spans="1:3">
+      <x:c r="A55" s="1" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B55">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="C55">
+        <x:v>109</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:3">
+      <x:c r="A56" s="1" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B56">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="C56">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:3">
+      <x:c r="A57" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="E31">
-        <x:f t="shared" si="3"/>
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F31">
-        <x:f t="shared" si="4"/>
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G31">
-        <x:f t="shared" si="5"/>
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:7">
-      <x:c r="A33" s="1"/>
-      <x:c r="B33" s="1"/>
-      <x:c r="C33" s="1"/>
-      <x:c r="D33" s="1"/>
-      <x:c r="E33" s="1"/>
-      <x:c r="F33" s="1"/>
-      <x:c r="G33" s="1"/>
-    </x:row>
-    <x:row r="34" spans="2:7">
-      <x:c r="B34" s="7" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C34" s="8"/>
-      <x:c r="D34" s="8"/>
-      <x:c r="E34" s="8"/>
-      <x:c r="F34" s="8"/>
-      <x:c r="G34" s="8"/>
-    </x:row>
-    <x:row r="35" spans="2:7">
-      <x:c r="B35" s="8"/>
-      <x:c r="C35" s="8"/>
-      <x:c r="D35" s="8"/>
-      <x:c r="E35" s="8"/>
-      <x:c r="F35" s="8"/>
-      <x:c r="G35" s="8"/>
-    </x:row>
-    <x:row r="36" spans="1:7">
-      <x:c r="A36" s="1"/>
-      <x:c r="B36" s="1" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C36" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D36" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="E36" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F36" s="1" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G36" s="1" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:7">
-      <x:c r="A37" s="1">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="B37">
-        <x:v>39530</x:v>
-      </x:c>
-      <x:c r="C37" s="1">
-        <x:v>39470</x:v>
-      </x:c>
-      <x:c r="D37" s="1">
-        <x:v>38000</x:v>
-      </x:c>
-      <x:c r="E37" s="1">
-        <x:v>34000</x:v>
-      </x:c>
-      <x:c r="F37" s="1">
-        <x:v>25100</x:v>
-      </x:c>
-      <x:c r="G37" s="1">
-        <x:v>21970</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:7">
-      <x:c r="A38" s="1">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="B38" s="1">
-        <x:v>36500</x:v>
-      </x:c>
-      <x:c r="C38" s="1">
-        <x:v>35600</x:v>
-      </x:c>
-      <x:c r="D38" s="1">
-        <x:v>32900</x:v>
-      </x:c>
-      <x:c r="E38" s="1">
-        <x:v>24270</x:v>
-      </x:c>
-      <x:c r="F38" s="1">
-        <x:v>18600</x:v>
-      </x:c>
-      <x:c r="G38" s="1">
-        <x:v>12700</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39" spans="1:7">
-      <x:c r="A39" s="1">
-        <x:v>128</x:v>
-      </x:c>
-      <x:c r="B39" s="1">
-        <x:v>31900</x:v>
-      </x:c>
-      <x:c r="C39" s="1">
-        <x:v>28400</x:v>
-      </x:c>
-      <x:c r="D39" s="1">
-        <x:v>22900</x:v>
-      </x:c>
-      <x:c r="E39" s="1">
-        <x:v>18200</x:v>
-      </x:c>
-      <x:c r="F39" s="1">
-        <x:v>9347</x:v>
-      </x:c>
-      <x:c r="G39" s="1">
-        <x:v>6363</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:7">
-      <x:c r="A40" s="1">
-        <x:v>256</x:v>
-      </x:c>
-      <x:c r="B40" s="1">
-        <x:v>25133</x:v>
-      </x:c>
-      <x:c r="C40" s="1">
-        <x:v>19800</x:v>
-      </x:c>
-      <x:c r="D40" s="1">
-        <x:v>17000</x:v>
-      </x:c>
-      <x:c r="E40" s="1">
-        <x:v>9170</x:v>
-      </x:c>
-      <x:c r="F40" s="1">
-        <x:v>4676</x:v>
-      </x:c>
-      <x:c r="G40" s="1">
-        <x:v>3183</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:7">
-      <x:c r="A41" s="1">
-        <x:v>512</x:v>
-      </x:c>
-      <x:c r="B41" s="1">
-        <x:v>16000</x:v>
-      </x:c>
-      <x:c r="C41" s="1">
-        <x:v>13600</x:v>
-      </x:c>
-      <x:c r="D41" s="1">
-        <x:v>8846</x:v>
-      </x:c>
-      <x:c r="E41" s="1">
-        <x:v>4589</x:v>
-      </x:c>
-      <x:c r="F41" s="1">
-        <x:v>2339</x:v>
-      </x:c>
-      <x:c r="G41" s="1">
-        <x:v>1592</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42" spans="1:7">
-      <x:c r="A42" s="1">
-        <x:v>1024</x:v>
-      </x:c>
-      <x:c r="B42" s="1">
-        <x:v>10425</x:v>
-      </x:c>
-      <x:c r="C42" s="1">
-        <x:v>8020</x:v>
-      </x:c>
-      <x:c r="D42" s="1">
-        <x:v>4423</x:v>
-      </x:c>
-      <x:c r="E42" s="1">
-        <x:v>2295</x:v>
-      </x:c>
-      <x:c r="F42" s="1">
-        <x:v>1169</x:v>
-      </x:c>
-      <x:c r="G42" s="1">
-        <x:v>796</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="1:7">
-      <x:c r="A43" s="1" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B43" s="1">
-        <x:v>5830</x:v>
-      </x:c>
-      <x:c r="C43" s="1">
-        <x:v>4113</x:v>
-      </x:c>
-      <x:c r="D43" s="1">
-        <x:v>2211</x:v>
-      </x:c>
-      <x:c r="E43" s="1">
-        <x:v>1147</x:v>
-      </x:c>
-      <x:c r="F43" s="1">
-        <x:v>585</x:v>
-      </x:c>
-      <x:c r="G43" s="1"/>
-    </x:row>
-    <x:row r="44" spans="1:7">
-      <x:c r="A44" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B44" s="1">
-        <x:v>2960</x:v>
-      </x:c>
-      <x:c r="C44" s="1">
-        <x:v>2020</x:v>
-      </x:c>
-      <x:c r="D44" s="1">
-        <x:v>1106</x:v>
-      </x:c>
-      <x:c r="E44" s="1">
-        <x:v>574</x:v>
-      </x:c>
-      <x:c r="F44" s="1"/>
-      <x:c r="G44" s="1"/>
-    </x:row>
-    <x:row r="45" spans="1:7">
-      <x:c r="A45" s="1" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B45" s="1">
-        <x:v>1490</x:v>
-      </x:c>
-      <x:c r="C45" s="1">
-        <x:v>1008</x:v>
-      </x:c>
-      <x:c r="D45" s="1">
-        <x:v>533</x:v>
-      </x:c>
-      <x:c r="E45" s="1"/>
-      <x:c r="F45" s="1"/>
-      <x:c r="G45" s="1"/>
-    </x:row>
-    <x:row r="46" spans="1:7">
-      <x:c r="A46" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B46" s="1">
-        <x:v>752</x:v>
-      </x:c>
-      <x:c r="C46" s="1">
-        <x:v>485</x:v>
-      </x:c>
-      <x:c r="D46" s="1"/>
-      <x:c r="E46" s="1"/>
-      <x:c r="F46" s="1"/>
-      <x:c r="G46" s="1"/>
-    </x:row>
-    <x:row r="47" spans="1:7">
-      <x:c r="A47" s="1" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="B47" s="1">
-        <x:v>384</x:v>
-      </x:c>
-      <x:c r="C47" s="1"/>
-      <x:c r="D47" s="1"/>
-      <x:c r="E47" s="1"/>
-      <x:c r="F47" s="1"/>
-      <x:c r="G47" s="1"/>
+      <x:c r="B57">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C57">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:2">
+      <x:c r="A58" s="1" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B58">
+        <x:v>22</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="3">
     <x:mergeCell ref="B1:G2"/>
-    <x:mergeCell ref="B18:G19"/>
-    <x:mergeCell ref="B34:G35"/>
+    <x:mergeCell ref="B21:G22"/>
+    <x:mergeCell ref="B41:G42"/>
   </x:mergeCells>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51166665554046631" footer="0.51166665554046631"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -9803,13 +9798,13 @@
   <x:sheetPr codeName="Sheet6"/>
   <x:dimension ref="A1:A1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <x:sheetView topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:selection activeCell="P61" activeCellId="0" sqref="P61:P61"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.550000000000001"/>
   <x:sheetData/>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51166665554046631" footer="0.51166665554046631"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <x:drawing r:id="rId1"/>
 </x:worksheet>

</xml_diff>